<commit_message>
on padister fan blue leds with clockwise display also added in exel file
</commit_message>
<xml_diff>
--- a/led pattren1.xlsx
+++ b/led pattren1.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10824" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10824" tabRatio="550" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="8bit pattren" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,6 +24,23 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>0b00000001,0b00000011,0b00000110,0b00001100,0b00000101,0b01111100,0b11000000,0b11000000,0b10111111,0b00000000,0b00110000,0b01001000,0b01111111,0b00000001,0b00011111,0b00000001,0b01111111,0b00000000,0b01111111</t>
+  </si>
+  <si>
+    <t>concatenate cells A-F</t>
+  </si>
+  <si>
+    <t>Convert to binary</t>
+  </si>
+  <si>
+    <t>convert to HEX</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -43,7 +61,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -74,8 +92,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -98,11 +134,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -113,6 +167,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -817,7 +890,7 @@
         <v>1</v>
       </c>
       <c r="P16" t="str">
-        <f t="shared" ref="P14:P16" si="0">MID(F22,1,8)</f>
+        <f t="shared" ref="P16" si="0">MID(F22,1,8)</f>
         <v/>
       </c>
     </row>
@@ -841,10 +914,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O82"/>
+  <dimension ref="A1:R82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -854,7 +927,7 @@
     <col min="9" max="15" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9">
         <v>1</v>
       </c>
@@ -902,8 +975,13 @@
         <f>CONCATENATE(G1,G2,G3,G4,G5,G6,G7,G8,G9,G10,G11,G12,G13,G14,G15,G16)</f>
         <v/>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -923,8 +1001,10 @@
         <v>0</v>
       </c>
       <c r="G2" s="7"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>1</v>
       </c>
@@ -945,35 +1025,40 @@
       </c>
       <c r="G3" s="7"/>
       <c r="I3" s="5" t="str">
-        <f>MID(I1,1,8)</f>
+        <f t="shared" ref="I3:O3" si="1">MID(I1,1,8)</f>
         <v>11111111</v>
       </c>
       <c r="J3" s="5" t="str">
-        <f>MID(J1,1,8)</f>
+        <f t="shared" si="1"/>
         <v>10010000</v>
       </c>
       <c r="K3" s="5" t="str">
-        <f>MID(K1,1,8)</f>
+        <f t="shared" si="1"/>
         <v>10010000</v>
       </c>
       <c r="L3" s="5" t="str">
-        <f>MID(L1,1,8)</f>
+        <f t="shared" si="1"/>
         <v>10010000</v>
       </c>
       <c r="M3" s="5" t="str">
-        <f>MID(M1,1,8)</f>
+        <f t="shared" si="1"/>
         <v>10000000</v>
       </c>
       <c r="N3" s="5" t="str">
-        <f>MID(N1,1,8)</f>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="O3" s="5" t="str">
-        <f>MID(O1,1,8)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -1001,7 +1086,7 @@
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>1</v>
       </c>
@@ -1022,35 +1107,40 @@
       </c>
       <c r="G5" s="7"/>
       <c r="I5" s="6" t="str">
-        <f>BIN2HEX(I3,2)</f>
+        <f t="shared" ref="I5:O5" si="2">BIN2HEX(I3,2)</f>
         <v>FF</v>
       </c>
       <c r="J5" s="6" t="str">
-        <f>BIN2HEX(J3,2)</f>
+        <f t="shared" si="2"/>
         <v>90</v>
       </c>
       <c r="K5" s="6" t="str">
-        <f>BIN2HEX(K3,2)</f>
+        <f t="shared" si="2"/>
         <v>90</v>
       </c>
       <c r="L5" s="6" t="str">
-        <f>BIN2HEX(L3,2)</f>
+        <f t="shared" si="2"/>
         <v>90</v>
       </c>
       <c r="M5" s="6" t="str">
-        <f>BIN2HEX(M3,2)</f>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
       <c r="N5" s="6" t="str">
-        <f>BIN2HEX(N3,2)</f>
+        <f t="shared" si="2"/>
         <v>00</v>
       </c>
       <c r="O5" s="6" t="str">
-        <f>BIN2HEX(O3,2)</f>
+        <f t="shared" si="2"/>
         <v>00</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P5" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>1</v>
       </c>
@@ -1071,31 +1161,31 @@
       </c>
       <c r="G6" s="7"/>
       <c r="I6" t="str">
-        <f>MID(I1,9,8)</f>
+        <f t="shared" ref="I6:N6" si="3">MID(I1,9,8)</f>
         <v/>
       </c>
       <c r="J6" t="str">
-        <f>MID(J1,9,8)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K6" t="str">
-        <f>MID(K1,9,8)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="L6" t="str">
-        <f>MID(L1,9,8)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M6" t="str">
-        <f>MID(M1,9,8)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N6" t="str">
-        <f>MID(N1,9,8)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>1</v>
       </c>
@@ -1116,27 +1206,27 @@
       </c>
       <c r="G7" s="7"/>
       <c r="I7" s="5" t="str">
-        <f>BIN2HEX(I6,2)</f>
+        <f t="shared" ref="I7:N7" si="4">BIN2HEX(I6,2)</f>
         <v>00</v>
       </c>
       <c r="J7" s="5" t="str">
-        <f>BIN2HEX(J6,2)</f>
+        <f t="shared" si="4"/>
         <v>00</v>
       </c>
       <c r="K7" s="5" t="str">
-        <f>BIN2HEX(K6,2)</f>
+        <f t="shared" si="4"/>
         <v>00</v>
       </c>
       <c r="L7" s="5" t="str">
-        <f>BIN2HEX(L6,2)</f>
+        <f t="shared" si="4"/>
         <v>00</v>
       </c>
       <c r="M7" s="5" t="str">
-        <f>BIN2HEX(M6,2)</f>
+        <f t="shared" si="4"/>
         <v>00</v>
       </c>
       <c r="N7" s="5" t="str">
-        <f>BIN2HEX(N6,2)</f>
+        <f t="shared" si="4"/>
         <v>00</v>
       </c>
       <c r="O7" s="5" t="str">
@@ -1144,7 +1234,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>1</v>
       </c>
@@ -1165,7 +1255,7 @@
       </c>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -1174,7 +1264,7 @@
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -1183,7 +1273,7 @@
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -1192,7 +1282,7 @@
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>0</v>
       </c>
@@ -1217,31 +1307,31 @@
         <v>01111111</v>
       </c>
       <c r="J12" t="str">
-        <f t="shared" ref="J12:O12" si="1">CONCATENATE(B12,B13,B14,B15,B16,B17,B18,B19)</f>
+        <f t="shared" ref="J12:O12" si="5">CONCATENATE(B12,B13,B14,B15,B16,B17,B18,B19)</f>
         <v>10001000</v>
       </c>
       <c r="K12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>10001000</v>
       </c>
       <c r="L12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>10001000</v>
       </c>
       <c r="M12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>01111111</v>
       </c>
       <c r="N12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>00000000</v>
       </c>
       <c r="O12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>1</v>
       </c>
@@ -1262,7 +1352,7 @@
       </c>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>1</v>
       </c>
@@ -1287,31 +1377,31 @@
         <v>01111111</v>
       </c>
       <c r="J14" s="5" t="str">
-        <f t="shared" ref="J14:O14" si="2">MID(J12,1,8)</f>
+        <f t="shared" ref="J14:O14" si="6">MID(J12,1,8)</f>
         <v>10001000</v>
       </c>
       <c r="K14" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>10001000</v>
       </c>
       <c r="L14" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>10001000</v>
       </c>
       <c r="M14" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>01111111</v>
       </c>
       <c r="N14" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>00000000</v>
       </c>
       <c r="O14" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>1</v>
       </c>
@@ -1332,7 +1422,7 @@
       </c>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>1</v>
       </c>
@@ -1357,27 +1447,27 @@
         <v>7F</v>
       </c>
       <c r="J16" s="6" t="str">
-        <f t="shared" ref="J16:O16" si="3">BIN2HEX(J14,2)</f>
+        <f t="shared" ref="J16:O16" si="7">BIN2HEX(J14,2)</f>
         <v>88</v>
       </c>
       <c r="K16" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>88</v>
       </c>
       <c r="L16" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>88</v>
       </c>
       <c r="M16" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>7F</v>
       </c>
       <c r="N16" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>00</v>
       </c>
       <c r="O16" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>00</v>
       </c>
     </row>
@@ -1465,27 +1555,27 @@
         <v>11111111</v>
       </c>
       <c r="J23" t="str">
-        <f t="shared" ref="J23:O23" si="4">CONCATENATE(B23,B24,B25,B26,B27,B28,B29,B30)</f>
+        <f t="shared" ref="J23:O23" si="8">CONCATENATE(B23,B24,B25,B26,B27,B28,B29,B30)</f>
         <v>10011000</v>
       </c>
       <c r="K23" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>10011100</v>
       </c>
       <c r="L23" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>10011010</v>
       </c>
       <c r="M23" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>11111001</v>
       </c>
       <c r="N23" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>00000000</v>
       </c>
       <c r="O23" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -1533,27 +1623,27 @@
         <v>11111111</v>
       </c>
       <c r="J25" s="5" t="str">
-        <f t="shared" ref="J25:O25" si="5">MID(J23,1,8)</f>
+        <f t="shared" ref="J25:O25" si="9">MID(J23,1,8)</f>
         <v>10011000</v>
       </c>
       <c r="K25" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>10011100</v>
       </c>
       <c r="L25" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>10011010</v>
       </c>
       <c r="M25" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>11111001</v>
       </c>
       <c r="N25" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>00000000</v>
       </c>
       <c r="O25" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
@@ -1601,27 +1691,27 @@
         <v>FF</v>
       </c>
       <c r="J27" s="6" t="str">
-        <f t="shared" ref="J27:O27" si="6">BIN2HEX(J25,2)</f>
+        <f t="shared" ref="J27:O27" si="10">BIN2HEX(J25,2)</f>
         <v>98</v>
       </c>
       <c r="K27" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>9C</v>
       </c>
       <c r="L27" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>9A</v>
       </c>
       <c r="M27" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>F9</v>
       </c>
       <c r="N27" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>00</v>
       </c>
       <c r="O27" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>00</v>
       </c>
     </row>
@@ -1709,27 +1799,27 @@
         <v>11111111</v>
       </c>
       <c r="J34" t="str">
-        <f t="shared" ref="J34:O34" si="7">CONCATENATE(B34,B35,B36,B37,B38,B39,B40,B41)</f>
+        <f t="shared" ref="J34:O34" si="11">CONCATENATE(B34,B35,B36,B37,B38,B39,B40,B41)</f>
         <v>00001000</v>
       </c>
       <c r="K34" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>00001000</v>
       </c>
       <c r="L34" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>00001000</v>
       </c>
       <c r="M34" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>11111111</v>
       </c>
       <c r="N34" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>00000000</v>
       </c>
       <c r="O34" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -1777,27 +1867,27 @@
         <v>11111111</v>
       </c>
       <c r="J36" s="5" t="str">
-        <f t="shared" ref="J36:O36" si="8">MID(J34,1,8)</f>
+        <f t="shared" ref="J36:O36" si="12">MID(J34,1,8)</f>
         <v>00001000</v>
       </c>
       <c r="K36" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>00001000</v>
       </c>
       <c r="L36" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>00001000</v>
       </c>
       <c r="M36" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>11111111</v>
       </c>
       <c r="N36" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>00000000</v>
       </c>
       <c r="O36" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
     </row>
@@ -1845,27 +1935,27 @@
         <v>FF</v>
       </c>
       <c r="J38" s="6" t="str">
-        <f t="shared" ref="J38:O38" si="9">BIN2HEX(J36,2)</f>
+        <f t="shared" ref="J38:O38" si="13">BIN2HEX(J36,2)</f>
         <v>08</v>
       </c>
       <c r="K38" s="6" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>08</v>
       </c>
       <c r="L38" s="6" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>08</v>
       </c>
       <c r="M38" s="6" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>FF</v>
       </c>
       <c r="N38" s="6" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>00</v>
       </c>
       <c r="O38" s="6" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>00</v>
       </c>
     </row>
@@ -1953,27 +2043,27 @@
         <v>01111111</v>
       </c>
       <c r="J44" t="str">
-        <f t="shared" ref="J44:O44" si="10">CONCATENATE(B44,B45,B46,B47,B48,B49,B50,B51)</f>
+        <f t="shared" ref="J44:O44" si="14">CONCATENATE(B44,B45,B46,B47,B48,B49,B50,B51)</f>
         <v>10001000</v>
       </c>
       <c r="K44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>10001000</v>
       </c>
       <c r="L44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>10001000</v>
       </c>
       <c r="M44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>10001000</v>
       </c>
       <c r="N44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>01111111</v>
       </c>
       <c r="O44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
@@ -2021,27 +2111,27 @@
         <v>01111111</v>
       </c>
       <c r="J46" s="5" t="str">
-        <f t="shared" ref="J46:O46" si="11">MID(J44,1,8)</f>
+        <f t="shared" ref="J46:O46" si="15">MID(J44,1,8)</f>
         <v>10001000</v>
       </c>
       <c r="K46" s="5" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>10001000</v>
       </c>
       <c r="L46" s="5" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>10001000</v>
       </c>
       <c r="M46" s="5" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>10001000</v>
       </c>
       <c r="N46" s="5" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>01111111</v>
       </c>
       <c r="O46" s="5" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
@@ -2089,27 +2179,27 @@
         <v>7F</v>
       </c>
       <c r="J48" s="6" t="str">
-        <f t="shared" ref="J48:O48" si="12">BIN2HEX(J46,2)</f>
+        <f t="shared" ref="J48:O48" si="16">BIN2HEX(J46,2)</f>
         <v>88</v>
       </c>
       <c r="K48" s="6" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>88</v>
       </c>
       <c r="L48" s="6" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>88</v>
       </c>
       <c r="M48" s="6" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>88</v>
       </c>
       <c r="N48" s="6" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>7F</v>
       </c>
       <c r="O48" s="6" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>00</v>
       </c>
     </row>
@@ -2197,27 +2287,27 @@
         <v>11111111</v>
       </c>
       <c r="J54" t="str">
-        <f t="shared" ref="J54:O54" si="13">CONCATENATE(B54,B55,B56,B57,B58,B59,B60,B61)</f>
+        <f t="shared" ref="J54:O54" si="17">CONCATENATE(B54,B55,B56,B57,B58,B59,B60,B61)</f>
         <v>11000000</v>
       </c>
       <c r="K54" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>00010000</v>
       </c>
       <c r="L54" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>00000100</v>
       </c>
       <c r="M54" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>11111111</v>
       </c>
       <c r="N54" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>00000000</v>
       </c>
       <c r="O54" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
@@ -2265,27 +2355,27 @@
         <v>11111111</v>
       </c>
       <c r="J56" s="5" t="str">
-        <f t="shared" ref="J56:O56" si="14">MID(J54,1,8)</f>
+        <f t="shared" ref="J56:O56" si="18">MID(J54,1,8)</f>
         <v>11000000</v>
       </c>
       <c r="K56" s="5" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>00010000</v>
       </c>
       <c r="L56" s="5" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>00000100</v>
       </c>
       <c r="M56" s="5" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>11111111</v>
       </c>
       <c r="N56" s="5" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>00000000</v>
       </c>
       <c r="O56" s="5" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
     </row>
@@ -2333,27 +2423,27 @@
         <v>FF</v>
       </c>
       <c r="J58" s="6" t="str">
-        <f t="shared" ref="J58:O58" si="15">BIN2HEX(J56,2)</f>
+        <f t="shared" ref="J58:O58" si="19">BIN2HEX(J56,2)</f>
         <v>C0</v>
       </c>
       <c r="K58" s="6" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>10</v>
       </c>
       <c r="L58" s="6" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>04</v>
       </c>
       <c r="M58" s="6" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>FF</v>
       </c>
       <c r="N58" s="6" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>00</v>
       </c>
       <c r="O58" s="6" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>00</v>
       </c>
     </row>
@@ -2441,27 +2531,27 @@
         <v>11111111</v>
       </c>
       <c r="J65" t="str">
-        <f t="shared" ref="J65:O65" si="16">CONCATENATE(B65,B66,B67,B68,B69,B70,B71,B72)</f>
+        <f t="shared" ref="J65:O65" si="20">CONCATENATE(B65,B66,B67,B68,B69,B70,B71,B72)</f>
         <v>10010000</v>
       </c>
       <c r="K65" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>10010000</v>
       </c>
       <c r="L65" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>10010000</v>
       </c>
       <c r="M65" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>10000000</v>
       </c>
       <c r="N65" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>00000000</v>
       </c>
       <c r="O65" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
     </row>
@@ -2509,27 +2599,27 @@
         <v>11111111</v>
       </c>
       <c r="J67" s="5" t="str">
-        <f t="shared" ref="J67:O67" si="17">MID(J65,1,8)</f>
+        <f t="shared" ref="J67:O67" si="21">MID(J65,1,8)</f>
         <v>10010000</v>
       </c>
       <c r="K67" s="5" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>10010000</v>
       </c>
       <c r="L67" s="5" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>10010000</v>
       </c>
       <c r="M67" s="5" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>10000000</v>
       </c>
       <c r="N67" s="5" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>00000000</v>
       </c>
       <c r="O67" s="5" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
@@ -2577,27 +2667,27 @@
         <v>FF</v>
       </c>
       <c r="J69" s="6" t="str">
-        <f t="shared" ref="J69:O69" si="18">BIN2HEX(J67,2)</f>
+        <f t="shared" ref="J69:O69" si="22">BIN2HEX(J67,2)</f>
         <v>90</v>
       </c>
       <c r="K69" s="6" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>90</v>
       </c>
       <c r="L69" s="6" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>90</v>
       </c>
       <c r="M69" s="6" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>80</v>
       </c>
       <c r="N69" s="6" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>00</v>
       </c>
       <c r="O69" s="6" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>00</v>
       </c>
     </row>
@@ -2685,27 +2775,27 @@
         <v>11111111</v>
       </c>
       <c r="J75" t="str">
-        <f t="shared" ref="J75:O75" si="19">CONCATENATE(B75,B76,B77,B78,B79,B80,B81,B82)</f>
+        <f t="shared" ref="J75:O75" si="23">CONCATENATE(B75,B76,B77,B78,B79,B80,B81,B82)</f>
         <v>10010000</v>
       </c>
       <c r="K75" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>10010000</v>
       </c>
       <c r="L75" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>10010000</v>
       </c>
       <c r="M75" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>10000000</v>
       </c>
       <c r="N75" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>00000000</v>
       </c>
       <c r="O75" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
@@ -2753,27 +2843,27 @@
         <v>11111111</v>
       </c>
       <c r="J77" s="5" t="str">
-        <f t="shared" ref="J77:O77" si="20">MID(J75,1,8)</f>
+        <f t="shared" ref="J77:O77" si="24">MID(J75,1,8)</f>
         <v>10010000</v>
       </c>
       <c r="K77" s="5" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>10010000</v>
       </c>
       <c r="L77" s="5" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>10010000</v>
       </c>
       <c r="M77" s="5" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>10000000</v>
       </c>
       <c r="N77" s="5" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>00000000</v>
       </c>
       <c r="O77" s="5" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
@@ -2821,27 +2911,27 @@
         <v>FF</v>
       </c>
       <c r="J79" s="6" t="str">
-        <f t="shared" ref="J79:O79" si="21">BIN2HEX(J77,2)</f>
+        <f t="shared" ref="J79:O79" si="25">BIN2HEX(J77,2)</f>
         <v>90</v>
       </c>
       <c r="K79" s="6" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>90</v>
       </c>
       <c r="L79" s="6" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>90</v>
       </c>
       <c r="M79" s="6" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>80</v>
       </c>
       <c r="N79" s="6" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>00</v>
       </c>
       <c r="O79" s="6" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>00</v>
       </c>
     </row>
@@ -2906,6 +2996,11 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="P5:R5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2913,10 +3008,186 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AN9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:AN9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="4.44140625" customWidth="1"/>
+    <col min="3" max="3" width="5.44140625" customWidth="1"/>
+    <col min="4" max="4" width="5" customWidth="1"/>
+    <col min="5" max="6" width="5.33203125" customWidth="1"/>
+    <col min="7" max="7" width="4.88671875" customWidth="1"/>
+    <col min="8" max="8" width="5.5546875" customWidth="1"/>
+    <col min="9" max="9" width="5" customWidth="1"/>
+    <col min="10" max="10" width="4.109375" customWidth="1"/>
+    <col min="11" max="11" width="4.77734375" customWidth="1"/>
+    <col min="12" max="13" width="4.44140625" customWidth="1"/>
+    <col min="14" max="14" width="4.21875" customWidth="1"/>
+    <col min="15" max="15" width="4" customWidth="1"/>
+    <col min="16" max="16" width="4.33203125" customWidth="1"/>
+    <col min="17" max="17" width="4.21875" customWidth="1"/>
+    <col min="18" max="18" width="4" customWidth="1"/>
+    <col min="19" max="19" width="4.33203125" customWidth="1"/>
+    <col min="20" max="20" width="4.21875" customWidth="1"/>
+    <col min="21" max="21" width="3.5546875" customWidth="1"/>
+    <col min="22" max="23" width="4.109375" customWidth="1"/>
+    <col min="24" max="24" width="4" customWidth="1"/>
+    <col min="25" max="25" width="3.21875" customWidth="1"/>
+    <col min="26" max="26" width="3.88671875" customWidth="1"/>
+    <col min="27" max="27" width="4.5546875" customWidth="1"/>
+    <col min="28" max="28" width="5.109375" customWidth="1"/>
+    <col min="29" max="29" width="4.6640625" customWidth="1"/>
+    <col min="30" max="30" width="5.21875" customWidth="1"/>
+    <col min="31" max="31" width="4.21875" customWidth="1"/>
+    <col min="32" max="32" width="4.33203125" customWidth="1"/>
+    <col min="33" max="34" width="4.6640625" customWidth="1"/>
+    <col min="35" max="35" width="4.5546875" customWidth="1"/>
+    <col min="36" max="36" width="4.109375" customWidth="1"/>
+    <col min="37" max="37" width="4.44140625" customWidth="1"/>
+    <col min="38" max="38" width="16.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="11"/>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="X2" s="11"/>
+      <c r="Y2" s="11"/>
+      <c r="AC2" s="12"/>
+      <c r="AD2" s="11"/>
+      <c r="AE2" s="11"/>
+      <c r="AI2" s="11"/>
+      <c r="AK2" s="10"/>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="X3" s="11"/>
+      <c r="AA3" s="11"/>
+      <c r="AC3" s="11"/>
+      <c r="AE3" s="11"/>
+      <c r="AI3" s="11"/>
+      <c r="AK3" s="10"/>
+    </row>
+    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="X4" s="11"/>
+      <c r="AA4" s="11"/>
+      <c r="AC4" s="11"/>
+      <c r="AE4" s="11"/>
+      <c r="AG4" s="11"/>
+      <c r="AI4" s="11"/>
+      <c r="AK4" s="10"/>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="V5" s="11"/>
+      <c r="X5" s="11"/>
+      <c r="AA5" s="11"/>
+      <c r="AC5" s="12"/>
+      <c r="AD5" s="11"/>
+      <c r="AE5" s="11"/>
+      <c r="AG5" s="11"/>
+      <c r="AI5" s="11"/>
+      <c r="AK5" s="10"/>
+    </row>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="11"/>
+      <c r="AA6" s="11"/>
+      <c r="AE6" s="11"/>
+      <c r="AG6" s="11"/>
+      <c r="AI6" s="11"/>
+      <c r="AK6" s="10"/>
+    </row>
+    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="12"/>
+      <c r="W7" s="12"/>
+      <c r="X7" s="12"/>
+      <c r="AA7" s="11"/>
+      <c r="AE7" s="11"/>
+      <c r="AG7" s="11"/>
+      <c r="AI7" s="11"/>
+      <c r="AK7" s="10"/>
+    </row>
+    <row r="8" spans="1:40" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+      <c r="W8" s="11"/>
+      <c r="AA8" s="11"/>
+      <c r="AE8" s="11"/>
+      <c r="AF8" s="11"/>
+      <c r="AG8" s="11"/>
+      <c r="AH8" s="11"/>
+      <c r="AI8" s="11"/>
+      <c r="AK8" s="10"/>
+    </row>
+    <row r="9" spans="1:40" ht="99" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13"/>
+      <c r="V9" s="13"/>
+      <c r="W9" s="13"/>
+      <c r="X9" s="13"/>
+      <c r="Y9" s="13"/>
+      <c r="Z9" s="13"/>
+      <c r="AA9" s="13"/>
+      <c r="AB9" s="13"/>
+      <c r="AC9" s="13"/>
+      <c r="AD9" s="13"/>
+      <c r="AE9" s="13"/>
+      <c r="AF9" s="13"/>
+      <c r="AG9" s="13"/>
+      <c r="AH9" s="13"/>
+      <c r="AI9" s="13"/>
+      <c r="AJ9" s="13"/>
+      <c r="AK9" s="13"/>
+      <c r="AL9" s="13"/>
+      <c r="AM9" s="13"/>
+      <c r="AN9" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A9:AN9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P25" sqref="A1:P25"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2949,31 +3220,31 @@
         <v>1</v>
       </c>
       <c r="I1" t="str">
-        <f>CONCATENATE(A1,A2,A3,A4,A5,A6,A7,A8,A9,A10,A11,A12,A13,A14,A15,A16)</f>
+        <f t="shared" ref="I1:O1" si="0">CONCATENATE(A1,A2,A3,A4,A5,A6,A7,A8,A9,A10,A11,A12,A13,A14,A15,A16)</f>
         <v>11111111</v>
       </c>
       <c r="J1" t="str">
-        <f>CONCATENATE(B1,B2,B3,B4,B5,B6,B7,B8,B9,B10,B11,B12,B13,B14,B15,B16)</f>
+        <f t="shared" si="0"/>
         <v>01111000</v>
       </c>
       <c r="K1" t="str">
-        <f>CONCATENATE(C1,C2,C3,C4,C5,C6,C7,C8,C9,C10,C11,C12,C13,C14,C15,C16)</f>
+        <f t="shared" si="0"/>
         <v>00000111</v>
       </c>
       <c r="L1" t="str">
-        <f>CONCATENATE(D1,D2,D3,D4,D5,D6,D7,D8,D9,D10,D11,D12,D13,D14,D15,D16)</f>
+        <f t="shared" si="0"/>
         <v>00000000</v>
       </c>
       <c r="M1" t="str">
-        <f>CONCATENATE(E1,E2,E3,E4,E5,E6,E7,E8,E9,E10,E11,E12,E13,E14,E15,E16)</f>
+        <f t="shared" si="0"/>
         <v>00000000</v>
       </c>
       <c r="N1" t="str">
-        <f>CONCATENATE(F1,F2,F3,F4,F5,F6,F7,F8,F9,F10,F11,F12,F13,F14,F15,F16)</f>
+        <f t="shared" si="0"/>
         <v>00000000</v>
       </c>
       <c r="O1" t="str">
-        <f>CONCATENATE(G1,G2,G3,G4,G5,G6,G7,G8,G9,G10,G11,G12,G13,G14,G15,G16)</f>
+        <f t="shared" si="0"/>
         <v>11111111</v>
       </c>
     </row>
@@ -3220,23 +3491,23 @@
         <v>01111000</v>
       </c>
       <c r="K18" s="5" t="str">
-        <f t="shared" ref="K18:O18" si="0">MID(K1,1,8)</f>
+        <f t="shared" ref="K18:O18" si="1">MID(K1,1,8)</f>
         <v>00000111</v>
       </c>
       <c r="L18" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="M18" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="N18" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
       <c r="O18" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11111111</v>
       </c>
     </row>
@@ -3251,31 +3522,31 @@
     </row>
     <row r="20" spans="9:15" x14ac:dyDescent="0.3">
       <c r="I20" s="5" t="str">
-        <f>BIN2HEX(I18,2)</f>
+        <f t="shared" ref="I20:O20" si="2">BIN2HEX(I18,2)</f>
         <v>FF</v>
       </c>
       <c r="J20" s="5" t="str">
-        <f>BIN2HEX(J18,2)</f>
+        <f t="shared" si="2"/>
         <v>78</v>
       </c>
       <c r="K20" s="5" t="str">
-        <f>BIN2HEX(K18,2)</f>
+        <f t="shared" si="2"/>
         <v>07</v>
       </c>
       <c r="L20" s="5" t="str">
-        <f>BIN2HEX(L18,2)</f>
+        <f t="shared" si="2"/>
         <v>00</v>
       </c>
       <c r="M20" s="5" t="str">
-        <f>BIN2HEX(M18,2)</f>
+        <f t="shared" si="2"/>
         <v>00</v>
       </c>
       <c r="N20" s="5" t="str">
-        <f>BIN2HEX(N18,2)</f>
+        <f t="shared" si="2"/>
         <v>00</v>
       </c>
       <c r="O20" s="5" t="str">
-        <f>BIN2HEX(O18,2)</f>
+        <f t="shared" si="2"/>
         <v>FF</v>
       </c>
     </row>
@@ -3285,27 +3556,27 @@
         <v/>
       </c>
       <c r="J23" t="str">
-        <f t="shared" ref="J23:O23" si="1">MID(J1,9,8)</f>
+        <f t="shared" ref="J23:O23" si="3">MID(J1,9,8)</f>
         <v/>
       </c>
       <c r="K23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="L23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="M23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="N23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="O23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -3315,27 +3586,27 @@
         <v>00</v>
       </c>
       <c r="J25" s="5" t="str">
-        <f t="shared" ref="J25:O25" si="2">BIN2HEX(J23,2)</f>
+        <f t="shared" ref="J25:O25" si="4">BIN2HEX(J23,2)</f>
         <v>00</v>
       </c>
       <c r="K25" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>00</v>
       </c>
       <c r="L25" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>00</v>
       </c>
       <c r="M25" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>00</v>
       </c>
       <c r="N25" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>00</v>
       </c>
       <c r="O25" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>00</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tested on harddisk version with fount added for all chrecters and moving the chrecters display postion for each chrecter
</commit_message>
<xml_diff>
--- a/led pattren1.xlsx
+++ b/led pattren1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10824" tabRatio="550" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10824" tabRatio="550" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
   <si>
     <t>0b00000001,0b00000011,0b00000110,0b00001100,0b00000101,0b01111100,0b11000000,0b11000000,0b10111111,0b00000000,0b00110000,0b01001000,0b01111111,0b00000001,0b00011111,0b00000001,0b01111111,0b00000000,0b01111111</t>
   </si>
@@ -39,6 +39,15 @@
   </si>
   <si>
     <t>convert to HEX</t>
+  </si>
+  <si>
+    <t>concatenate cells A-F-for reverse cell one is LSB</t>
+  </si>
+  <si>
+    <t>Anti clockwise</t>
+  </si>
+  <si>
+    <t>clockwise</t>
   </si>
 </sst>
 </file>
@@ -61,7 +70,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -107,6 +116,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -156,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -170,20 +191,26 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -914,10 +941,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R82"/>
+  <dimension ref="A1:V82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -927,7 +954,7 @@
     <col min="9" max="15" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9">
         <v>1</v>
       </c>
@@ -947,41 +974,45 @@
         <v>0</v>
       </c>
       <c r="G1" s="7"/>
-      <c r="I1" t="str">
-        <f>CONCATENATE(A1,A2,A3,A4,A5,A6,A7,A8)</f>
+      <c r="I1" s="19" t="str">
+        <f t="shared" ref="I1:N1" si="0">CONCATENATE(A1,A2,A3,A4,A5,A6,A7,A8)</f>
         <v>11111111</v>
       </c>
-      <c r="J1" t="str">
-        <f t="shared" ref="J1:N1" si="0">CONCATENATE(B1,B2,B3,B4,B5,B6,B7,B8)</f>
-        <v>10010000</v>
-      </c>
-      <c r="K1" t="str">
+      <c r="J1" s="19" t="str">
         <f t="shared" si="0"/>
         <v>10010000</v>
       </c>
-      <c r="L1" t="str">
+      <c r="K1" s="19" t="str">
         <f t="shared" si="0"/>
         <v>10010000</v>
       </c>
-      <c r="M1" t="str">
+      <c r="L1" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>10010000</v>
+      </c>
+      <c r="M1" s="19" t="str">
         <f t="shared" si="0"/>
         <v>10000000</v>
       </c>
-      <c r="N1" t="str">
+      <c r="N1" s="19" t="str">
         <f t="shared" si="0"/>
         <v>00000000</v>
       </c>
-      <c r="O1" t="str">
+      <c r="O1" s="19" t="str">
         <f>CONCATENATE(G1,G2,G3,G4,G5,G6,G7,G8,G9,G10,G11,G12,G13,G14,G15,G16)</f>
         <v/>
       </c>
-      <c r="P1" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P1" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="U1" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="V1" s="17"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -1001,10 +1032,44 @@
         <v>0</v>
       </c>
       <c r="G2" s="7"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="I2" s="18" t="str">
+        <f>CONCATENATE(A8,A7,A6,A5,A4,A3,A2,A1)</f>
+        <v>11111111</v>
+      </c>
+      <c r="J2" s="18" t="str">
+        <f t="shared" ref="J2:N2" si="1">CONCATENATE(B8,B7,B6,B5,B4,B3,B2,B1)</f>
+        <v>00001001</v>
+      </c>
+      <c r="K2" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>00001001</v>
+      </c>
+      <c r="L2" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>00001001</v>
+      </c>
+      <c r="M2" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>00000001</v>
+      </c>
+      <c r="N2" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>00000000</v>
+      </c>
+      <c r="O2" s="18"/>
+      <c r="P2" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
+      <c r="U2" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="V2" s="17"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>1</v>
       </c>
@@ -1025,40 +1090,44 @@
       </c>
       <c r="G3" s="7"/>
       <c r="I3" s="5" t="str">
-        <f t="shared" ref="I3:O3" si="1">MID(I1,1,8)</f>
+        <f t="shared" ref="I3:O4" si="2">MID(I1,1,8)</f>
         <v>11111111</v>
       </c>
       <c r="J3" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10010000</v>
       </c>
       <c r="K3" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10010000</v>
       </c>
       <c r="L3" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10010000</v>
       </c>
       <c r="M3" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10000000</v>
       </c>
       <c r="N3" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>00000000</v>
       </c>
       <c r="O3" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="P3" s="17" t="s">
+      <c r="P3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="U3" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="V3" s="17"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -1078,15 +1147,44 @@
         <v>0</v>
       </c>
       <c r="G4" s="7"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="I4" s="18" t="str">
+        <f>MID(I2,1,8)</f>
+        <v>11111111</v>
+      </c>
+      <c r="J4" s="18" t="str">
+        <f t="shared" ref="J4:N4" si="3">MID(J2,1,8)</f>
+        <v>00001001</v>
+      </c>
+      <c r="K4" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>00001001</v>
+      </c>
+      <c r="L4" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>00001001</v>
+      </c>
+      <c r="M4" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>00000001</v>
+      </c>
+      <c r="N4" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>00000000</v>
+      </c>
+      <c r="O4" s="18"/>
+      <c r="P4" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="V4" s="17"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>1</v>
       </c>
@@ -1107,134 +1205,132 @@
       </c>
       <c r="G5" s="7"/>
       <c r="I5" s="6" t="str">
-        <f t="shared" ref="I5:O5" si="2">BIN2HEX(I3,2)</f>
+        <f t="shared" ref="I5:O6" si="4">BIN2HEX(I3,2)</f>
         <v>FF</v>
       </c>
       <c r="J5" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>90</v>
       </c>
       <c r="K5" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>90</v>
       </c>
       <c r="L5" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>90</v>
       </c>
       <c r="M5" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>80</v>
       </c>
       <c r="N5" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>00</v>
-      </c>
-      <c r="O5" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>00</v>
-      </c>
-      <c r="P5" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="16"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="9">
-        <v>1</v>
-      </c>
-      <c r="B6" s="3">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0</v>
-      </c>
-      <c r="G6" s="7"/>
-      <c r="I6" t="str">
-        <f t="shared" ref="I6:N6" si="3">MID(I1,9,8)</f>
-        <v/>
-      </c>
-      <c r="J6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="L6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="M6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="N6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="9">
-        <v>1</v>
-      </c>
-      <c r="B7" s="3">
-        <v>0</v>
-      </c>
-      <c r="C7" s="3">
-        <v>0</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0</v>
-      </c>
-      <c r="G7" s="7"/>
-      <c r="I7" s="5" t="str">
-        <f t="shared" ref="I7:N7" si="4">BIN2HEX(I6,2)</f>
-        <v>00</v>
-      </c>
-      <c r="J7" s="5" t="str">
         <f t="shared" si="4"/>
         <v>00</v>
       </c>
-      <c r="K7" s="5" t="str">
+      <c r="O5" s="6" t="str">
         <f t="shared" si="4"/>
         <v>00</v>
       </c>
-      <c r="L7" s="5" t="str">
+      <c r="P5" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="U5" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="V5" s="17"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A6" s="9">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="7"/>
+      <c r="I6" s="20" t="str">
+        <f t="shared" si="4"/>
+        <v>FF</v>
+      </c>
+      <c r="J6" s="20" t="str">
+        <f t="shared" si="4"/>
+        <v>09</v>
+      </c>
+      <c r="K6" s="20" t="str">
+        <f t="shared" si="4"/>
+        <v>09</v>
+      </c>
+      <c r="L6" s="20" t="str">
+        <f t="shared" si="4"/>
+        <v>09</v>
+      </c>
+      <c r="M6" s="20" t="str">
+        <f t="shared" si="4"/>
+        <v>01</v>
+      </c>
+      <c r="N6" s="20" t="str">
         <f t="shared" si="4"/>
         <v>00</v>
       </c>
-      <c r="M7" s="5" t="str">
+      <c r="O6" s="20" t="str">
         <f t="shared" si="4"/>
         <v>00</v>
       </c>
-      <c r="N7" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>00</v>
-      </c>
-      <c r="O7" s="5" t="str">
-        <f>BIN2HEX(O23,2)</f>
-        <v>00</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P6" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="17"/>
+      <c r="U6" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="V6" s="17"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A7" s="9">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>1</v>
       </c>
@@ -1255,7 +1351,7 @@
       </c>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -1264,7 +1360,7 @@
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -1273,7 +1369,7 @@
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -1282,7 +1378,7 @@
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>0</v>
       </c>
@@ -1331,7 +1427,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>1</v>
       </c>
@@ -1351,8 +1447,32 @@
         <v>0</v>
       </c>
       <c r="G13" s="8"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="I13" s="18" t="str">
+        <f>CONCATENATE(A19,A18,A17,A16,A15,A14,A13,A12)</f>
+        <v>11111110</v>
+      </c>
+      <c r="J13" s="18" t="str">
+        <f t="shared" ref="J13:N13" si="6">CONCATENATE(B19,B18,B17,B16,B15,B14,B13,B12)</f>
+        <v>00010001</v>
+      </c>
+      <c r="K13" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>00010001</v>
+      </c>
+      <c r="L13" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>00010001</v>
+      </c>
+      <c r="M13" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>11111110</v>
+      </c>
+      <c r="N13" s="18" t="str">
+        <f t="shared" si="6"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>1</v>
       </c>
@@ -1377,31 +1497,31 @@
         <v>01111111</v>
       </c>
       <c r="J14" s="5" t="str">
-        <f t="shared" ref="J14:O14" si="6">MID(J12,1,8)</f>
+        <f t="shared" ref="J14:O14" si="7">MID(J12,1,8)</f>
         <v>10001000</v>
       </c>
       <c r="K14" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10001000</v>
       </c>
       <c r="L14" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10001000</v>
       </c>
       <c r="M14" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>01111111</v>
       </c>
       <c r="N14" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>00000000</v>
       </c>
       <c r="O14" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>1</v>
       </c>
@@ -1421,8 +1541,32 @@
         <v>0</v>
       </c>
       <c r="G15" s="8"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="I15" s="18" t="str">
+        <f>MID(I13,1,8)</f>
+        <v>11111110</v>
+      </c>
+      <c r="J15" s="18" t="str">
+        <f t="shared" ref="J15:N15" si="8">MID(J13,1,8)</f>
+        <v>00010001</v>
+      </c>
+      <c r="K15" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v>00010001</v>
+      </c>
+      <c r="L15" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v>00010001</v>
+      </c>
+      <c r="M15" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v>11111110</v>
+      </c>
+      <c r="N15" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>1</v>
       </c>
@@ -1447,27 +1591,27 @@
         <v>7F</v>
       </c>
       <c r="J16" s="6" t="str">
-        <f t="shared" ref="J16:O16" si="7">BIN2HEX(J14,2)</f>
+        <f t="shared" ref="J16:O16" si="9">BIN2HEX(J14,2)</f>
         <v>88</v>
       </c>
       <c r="K16" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>88</v>
       </c>
       <c r="L16" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>88</v>
       </c>
       <c r="M16" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>7F</v>
       </c>
       <c r="N16" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>00</v>
       </c>
       <c r="O16" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>00</v>
       </c>
     </row>
@@ -1489,6 +1633,30 @@
       </c>
       <c r="F17" s="3">
         <v>0</v>
+      </c>
+      <c r="I17" s="21" t="str">
+        <f t="shared" ref="I17:N17" si="10">BIN2HEX(I15,2)</f>
+        <v>FE</v>
+      </c>
+      <c r="J17" s="21" t="str">
+        <f t="shared" si="10"/>
+        <v>11</v>
+      </c>
+      <c r="K17" s="21" t="str">
+        <f t="shared" si="10"/>
+        <v>11</v>
+      </c>
+      <c r="L17" s="21" t="str">
+        <f t="shared" si="10"/>
+        <v>11</v>
+      </c>
+      <c r="M17" s="21" t="str">
+        <f t="shared" si="10"/>
+        <v>FE</v>
+      </c>
+      <c r="N17" s="21" t="str">
+        <f t="shared" si="10"/>
+        <v>00</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
@@ -1555,27 +1723,27 @@
         <v>11111111</v>
       </c>
       <c r="J23" t="str">
-        <f t="shared" ref="J23:O23" si="8">CONCATENATE(B23,B24,B25,B26,B27,B28,B29,B30)</f>
+        <f t="shared" ref="J23" si="11">CONCATENATE(B23,B24,B25,B26,B27,B28,B29,B30)</f>
         <v>10011000</v>
       </c>
       <c r="K23" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="K23" si="12">CONCATENATE(C23,C24,C25,C26,C27,C28,C29,C30)</f>
         <v>10011100</v>
       </c>
       <c r="L23" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="L23" si="13">CONCATENATE(D23,D24,D25,D26,D27,D28,D29,D30)</f>
         <v>10011010</v>
       </c>
       <c r="M23" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="M23" si="14">CONCATENATE(E23,E24,E25,E26,E27,E28,E29,E30)</f>
         <v>11111001</v>
       </c>
       <c r="N23" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="N23" si="15">CONCATENATE(F23,F24,F25,F26,F27,F28,F29,F30)</f>
         <v>00000000</v>
       </c>
       <c r="O23" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="O23" si="16">CONCATENATE(G23,G24,G25,G26,G27,G28,G29,G30)</f>
         <v/>
       </c>
     </row>
@@ -1597,6 +1765,30 @@
       </c>
       <c r="F24" s="3">
         <v>0</v>
+      </c>
+      <c r="I24" s="18" t="str">
+        <f>CONCATENATE(A30,A29,A28,A27,A26,A25,A24,A23)</f>
+        <v>11111111</v>
+      </c>
+      <c r="J24" s="18" t="str">
+        <f t="shared" ref="J24" si="17">CONCATENATE(B30,B29,B28,B27,B26,B25,B24,B23)</f>
+        <v>00011001</v>
+      </c>
+      <c r="K24" s="18" t="str">
+        <f t="shared" ref="K24" si="18">CONCATENATE(C30,C29,C28,C27,C26,C25,C24,C23)</f>
+        <v>00111001</v>
+      </c>
+      <c r="L24" s="18" t="str">
+        <f t="shared" ref="L24" si="19">CONCATENATE(D30,D29,D28,D27,D26,D25,D24,D23)</f>
+        <v>01011001</v>
+      </c>
+      <c r="M24" s="18" t="str">
+        <f t="shared" ref="M24" si="20">CONCATENATE(E30,E29,E28,E27,E26,E25,E24,E23)</f>
+        <v>10011111</v>
+      </c>
+      <c r="N24" s="18" t="str">
+        <f t="shared" ref="N24" si="21">CONCATENATE(F30,F29,F28,F27,F26,F25,F24,F23)</f>
+        <v>00000000</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -1623,27 +1815,27 @@
         <v>11111111</v>
       </c>
       <c r="J25" s="5" t="str">
-        <f t="shared" ref="J25:O25" si="9">MID(J23,1,8)</f>
+        <f t="shared" ref="J25:O25" si="22">MID(J23,1,8)</f>
         <v>10011000</v>
       </c>
       <c r="K25" s="5" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>10011100</v>
       </c>
       <c r="L25" s="5" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>10011010</v>
       </c>
       <c r="M25" s="5" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>11111001</v>
       </c>
       <c r="N25" s="5" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>00000000</v>
       </c>
       <c r="O25" s="5" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
     </row>
@@ -1665,6 +1857,30 @@
       </c>
       <c r="F26" s="3">
         <v>0</v>
+      </c>
+      <c r="I26" s="18" t="str">
+        <f>MID(I24,1,8)</f>
+        <v>11111111</v>
+      </c>
+      <c r="J26" s="18" t="str">
+        <f t="shared" ref="J26:N26" si="23">MID(J24,1,8)</f>
+        <v>00011001</v>
+      </c>
+      <c r="K26" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v>00111001</v>
+      </c>
+      <c r="L26" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v>01011001</v>
+      </c>
+      <c r="M26" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v>10011111</v>
+      </c>
+      <c r="N26" s="18" t="str">
+        <f t="shared" si="23"/>
+        <v>00000000</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
@@ -1691,27 +1907,27 @@
         <v>FF</v>
       </c>
       <c r="J27" s="6" t="str">
-        <f t="shared" ref="J27:O27" si="10">BIN2HEX(J25,2)</f>
+        <f t="shared" ref="J27:O27" si="24">BIN2HEX(J25,2)</f>
         <v>98</v>
       </c>
       <c r="K27" s="6" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="24"/>
         <v>9C</v>
       </c>
       <c r="L27" s="6" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="24"/>
         <v>9A</v>
       </c>
       <c r="M27" s="6" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="24"/>
         <v>F9</v>
       </c>
       <c r="N27" s="6" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="24"/>
         <v>00</v>
       </c>
       <c r="O27" s="6" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="24"/>
         <v>00</v>
       </c>
     </row>
@@ -1733,6 +1949,30 @@
       </c>
       <c r="F28" s="3">
         <v>0</v>
+      </c>
+      <c r="I28" s="21" t="str">
+        <f t="shared" ref="I28:N28" si="25">BIN2HEX(I26,2)</f>
+        <v>FF</v>
+      </c>
+      <c r="J28" s="21" t="str">
+        <f t="shared" si="25"/>
+        <v>19</v>
+      </c>
+      <c r="K28" s="21" t="str">
+        <f t="shared" si="25"/>
+        <v>39</v>
+      </c>
+      <c r="L28" s="21" t="str">
+        <f t="shared" si="25"/>
+        <v>59</v>
+      </c>
+      <c r="M28" s="21" t="str">
+        <f t="shared" si="25"/>
+        <v>9F</v>
+      </c>
+      <c r="N28" s="21" t="str">
+        <f t="shared" si="25"/>
+        <v>00</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
@@ -1799,27 +2039,27 @@
         <v>11111111</v>
       </c>
       <c r="J34" t="str">
-        <f t="shared" ref="J34:O34" si="11">CONCATENATE(B34,B35,B36,B37,B38,B39,B40,B41)</f>
+        <f t="shared" ref="J34" si="26">CONCATENATE(B34,B35,B36,B37,B38,B39,B40,B41)</f>
         <v>00001000</v>
       </c>
       <c r="K34" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="K34" si="27">CONCATENATE(C34,C35,C36,C37,C38,C39,C40,C41)</f>
         <v>00001000</v>
       </c>
       <c r="L34" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="L34" si="28">CONCATENATE(D34,D35,D36,D37,D38,D39,D40,D41)</f>
         <v>00001000</v>
       </c>
       <c r="M34" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="M34" si="29">CONCATENATE(E34,E35,E36,E37,E38,E39,E40,E41)</f>
         <v>11111111</v>
       </c>
       <c r="N34" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="N34" si="30">CONCATENATE(F34,F35,F36,F37,F38,F39,F40,F41)</f>
         <v>00000000</v>
       </c>
       <c r="O34" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="O34" si="31">CONCATENATE(G34,G35,G36,G37,G38,G39,G40,G41)</f>
         <v/>
       </c>
     </row>
@@ -1841,6 +2081,30 @@
       </c>
       <c r="F35" s="9">
         <v>0</v>
+      </c>
+      <c r="I35" s="18" t="str">
+        <f>CONCATENATE(A41,A40,A39,A38,A37,A36,A35,A34)</f>
+        <v>11111111</v>
+      </c>
+      <c r="J35" s="18" t="str">
+        <f t="shared" ref="J35" si="32">CONCATENATE(B41,B40,B39,B38,B37,B36,B35,B34)</f>
+        <v>00010000</v>
+      </c>
+      <c r="K35" s="18" t="str">
+        <f t="shared" ref="K35" si="33">CONCATENATE(C41,C40,C39,C38,C37,C36,C35,C34)</f>
+        <v>00010000</v>
+      </c>
+      <c r="L35" s="18" t="str">
+        <f t="shared" ref="L35" si="34">CONCATENATE(D41,D40,D39,D38,D37,D36,D35,D34)</f>
+        <v>00010000</v>
+      </c>
+      <c r="M35" s="18" t="str">
+        <f t="shared" ref="M35" si="35">CONCATENATE(E41,E40,E39,E38,E37,E36,E35,E34)</f>
+        <v>11111111</v>
+      </c>
+      <c r="N35" s="18" t="str">
+        <f t="shared" ref="N35" si="36">CONCATENATE(F41,F40,F39,F38,F37,F36,F35,F34)</f>
+        <v>00000000</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
@@ -1867,27 +2131,27 @@
         <v>11111111</v>
       </c>
       <c r="J36" s="5" t="str">
-        <f t="shared" ref="J36:O36" si="12">MID(J34,1,8)</f>
+        <f t="shared" ref="J36:O36" si="37">MID(J34,1,8)</f>
         <v>00001000</v>
       </c>
       <c r="K36" s="5" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="37"/>
         <v>00001000</v>
       </c>
       <c r="L36" s="5" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="37"/>
         <v>00001000</v>
       </c>
       <c r="M36" s="5" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="37"/>
         <v>11111111</v>
       </c>
       <c r="N36" s="5" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="37"/>
         <v>00000000</v>
       </c>
       <c r="O36" s="5" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="37"/>
         <v/>
       </c>
     </row>
@@ -1909,6 +2173,30 @@
       </c>
       <c r="F37" s="9">
         <v>0</v>
+      </c>
+      <c r="I37" s="18" t="str">
+        <f>MID(I35,1,8)</f>
+        <v>11111111</v>
+      </c>
+      <c r="J37" s="18" t="str">
+        <f t="shared" ref="J37:N37" si="38">MID(J35,1,8)</f>
+        <v>00010000</v>
+      </c>
+      <c r="K37" s="18" t="str">
+        <f t="shared" si="38"/>
+        <v>00010000</v>
+      </c>
+      <c r="L37" s="18" t="str">
+        <f t="shared" si="38"/>
+        <v>00010000</v>
+      </c>
+      <c r="M37" s="18" t="str">
+        <f t="shared" si="38"/>
+        <v>11111111</v>
+      </c>
+      <c r="N37" s="18" t="str">
+        <f t="shared" si="38"/>
+        <v>00000000</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
@@ -1935,27 +2223,27 @@
         <v>FF</v>
       </c>
       <c r="J38" s="6" t="str">
-        <f t="shared" ref="J38:O38" si="13">BIN2HEX(J36,2)</f>
+        <f t="shared" ref="J38:O38" si="39">BIN2HEX(J36,2)</f>
         <v>08</v>
       </c>
       <c r="K38" s="6" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="39"/>
         <v>08</v>
       </c>
       <c r="L38" s="6" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="39"/>
         <v>08</v>
       </c>
       <c r="M38" s="6" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="39"/>
         <v>FF</v>
       </c>
       <c r="N38" s="6" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="39"/>
         <v>00</v>
       </c>
       <c r="O38" s="6" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="39"/>
         <v>00</v>
       </c>
     </row>
@@ -1977,6 +2265,30 @@
       </c>
       <c r="F39" s="9">
         <v>0</v>
+      </c>
+      <c r="I39" s="21" t="str">
+        <f t="shared" ref="I39:N39" si="40">BIN2HEX(I37,2)</f>
+        <v>FF</v>
+      </c>
+      <c r="J39" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v>10</v>
+      </c>
+      <c r="K39" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v>10</v>
+      </c>
+      <c r="L39" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v>10</v>
+      </c>
+      <c r="M39" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v>FF</v>
+      </c>
+      <c r="N39" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v>00</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.3">
@@ -2043,27 +2355,27 @@
         <v>01111111</v>
       </c>
       <c r="J44" t="str">
-        <f t="shared" ref="J44:O44" si="14">CONCATENATE(B44,B45,B46,B47,B48,B49,B50,B51)</f>
+        <f t="shared" ref="J44" si="41">CONCATENATE(B44,B45,B46,B47,B48,B49,B50,B51)</f>
         <v>10001000</v>
       </c>
       <c r="K44" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="K44" si="42">CONCATENATE(C44,C45,C46,C47,C48,C49,C50,C51)</f>
         <v>10001000</v>
       </c>
       <c r="L44" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="L44" si="43">CONCATENATE(D44,D45,D46,D47,D48,D49,D50,D51)</f>
         <v>10001000</v>
       </c>
       <c r="M44" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="M44" si="44">CONCATENATE(E44,E45,E46,E47,E48,E49,E50,E51)</f>
         <v>10001000</v>
       </c>
       <c r="N44" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="N44" si="45">CONCATENATE(F44,F45,F46,F47,F48,F49,F50,F51)</f>
         <v>01111111</v>
       </c>
       <c r="O44" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="O44" si="46">CONCATENATE(G44,G45,G46,G47,G48,G49,G50,G51)</f>
         <v/>
       </c>
     </row>
@@ -2085,6 +2397,30 @@
       </c>
       <c r="F45" s="9">
         <v>1</v>
+      </c>
+      <c r="I45" s="18" t="str">
+        <f>CONCATENATE(A51,A50,A49,A48,A47,A46,A45,A44)</f>
+        <v>11111110</v>
+      </c>
+      <c r="J45" s="18" t="str">
+        <f t="shared" ref="J45" si="47">CONCATENATE(B51,B50,B49,B48,B47,B46,B45,B44)</f>
+        <v>00010001</v>
+      </c>
+      <c r="K45" s="18" t="str">
+        <f t="shared" ref="K45" si="48">CONCATENATE(C51,C50,C49,C48,C47,C46,C45,C44)</f>
+        <v>00010001</v>
+      </c>
+      <c r="L45" s="18" t="str">
+        <f t="shared" ref="L45" si="49">CONCATENATE(D51,D50,D49,D48,D47,D46,D45,D44)</f>
+        <v>00010001</v>
+      </c>
+      <c r="M45" s="18" t="str">
+        <f t="shared" ref="M45" si="50">CONCATENATE(E51,E50,E49,E48,E47,E46,E45,E44)</f>
+        <v>00010001</v>
+      </c>
+      <c r="N45" s="18" t="str">
+        <f t="shared" ref="N45" si="51">CONCATENATE(F51,F50,F49,F48,F47,F46,F45,F44)</f>
+        <v>11111110</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.3">
@@ -2111,27 +2447,27 @@
         <v>01111111</v>
       </c>
       <c r="J46" s="5" t="str">
-        <f t="shared" ref="J46:O46" si="15">MID(J44,1,8)</f>
+        <f t="shared" ref="J46:O46" si="52">MID(J44,1,8)</f>
         <v>10001000</v>
       </c>
       <c r="K46" s="5" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="52"/>
         <v>10001000</v>
       </c>
       <c r="L46" s="5" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="52"/>
         <v>10001000</v>
       </c>
       <c r="M46" s="5" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="52"/>
         <v>10001000</v>
       </c>
       <c r="N46" s="5" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="52"/>
         <v>01111111</v>
       </c>
       <c r="O46" s="5" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="52"/>
         <v/>
       </c>
     </row>
@@ -2153,6 +2489,30 @@
       </c>
       <c r="F47" s="9">
         <v>1</v>
+      </c>
+      <c r="I47" s="18" t="str">
+        <f>MID(I45,1,8)</f>
+        <v>11111110</v>
+      </c>
+      <c r="J47" s="18" t="str">
+        <f t="shared" ref="J47:N47" si="53">MID(J45,1,8)</f>
+        <v>00010001</v>
+      </c>
+      <c r="K47" s="18" t="str">
+        <f t="shared" si="53"/>
+        <v>00010001</v>
+      </c>
+      <c r="L47" s="18" t="str">
+        <f t="shared" si="53"/>
+        <v>00010001</v>
+      </c>
+      <c r="M47" s="18" t="str">
+        <f t="shared" si="53"/>
+        <v>00010001</v>
+      </c>
+      <c r="N47" s="18" t="str">
+        <f t="shared" si="53"/>
+        <v>11111110</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.3">
@@ -2179,27 +2539,27 @@
         <v>7F</v>
       </c>
       <c r="J48" s="6" t="str">
-        <f t="shared" ref="J48:O48" si="16">BIN2HEX(J46,2)</f>
+        <f t="shared" ref="J48:O48" si="54">BIN2HEX(J46,2)</f>
         <v>88</v>
       </c>
       <c r="K48" s="6" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="54"/>
         <v>88</v>
       </c>
       <c r="L48" s="6" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="54"/>
         <v>88</v>
       </c>
       <c r="M48" s="6" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="54"/>
         <v>88</v>
       </c>
       <c r="N48" s="6" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="54"/>
         <v>7F</v>
       </c>
       <c r="O48" s="6" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="54"/>
         <v>00</v>
       </c>
     </row>
@@ -2221,6 +2581,30 @@
       </c>
       <c r="F49" s="9">
         <v>1</v>
+      </c>
+      <c r="I49" s="21" t="str">
+        <f t="shared" ref="I49:N49" si="55">BIN2HEX(I47,2)</f>
+        <v>FE</v>
+      </c>
+      <c r="J49" s="21" t="str">
+        <f t="shared" si="55"/>
+        <v>11</v>
+      </c>
+      <c r="K49" s="21" t="str">
+        <f t="shared" si="55"/>
+        <v>11</v>
+      </c>
+      <c r="L49" s="21" t="str">
+        <f t="shared" si="55"/>
+        <v>11</v>
+      </c>
+      <c r="M49" s="21" t="str">
+        <f t="shared" si="55"/>
+        <v>11</v>
+      </c>
+      <c r="N49" s="21" t="str">
+        <f t="shared" si="55"/>
+        <v>FE</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.3">
@@ -2287,27 +2671,27 @@
         <v>11111111</v>
       </c>
       <c r="J54" t="str">
-        <f t="shared" ref="J54:O54" si="17">CONCATENATE(B54,B55,B56,B57,B58,B59,B60,B61)</f>
+        <f t="shared" ref="J54" si="56">CONCATENATE(B54,B55,B56,B57,B58,B59,B60,B61)</f>
         <v>11000000</v>
       </c>
       <c r="K54" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="K54" si="57">CONCATENATE(C54,C55,C56,C57,C58,C59,C60,C61)</f>
         <v>00010000</v>
       </c>
       <c r="L54" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="L54" si="58">CONCATENATE(D54,D55,D56,D57,D58,D59,D60,D61)</f>
         <v>00000100</v>
       </c>
       <c r="M54" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="M54" si="59">CONCATENATE(E54,E55,E56,E57,E58,E59,E60,E61)</f>
         <v>11111111</v>
       </c>
       <c r="N54" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="N54" si="60">CONCATENATE(F54,F55,F56,F57,F58,F59,F60,F61)</f>
         <v>00000000</v>
       </c>
       <c r="O54" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="O54" si="61">CONCATENATE(G54,G55,G56,G57,G58,G59,G60,G61)</f>
         <v/>
       </c>
     </row>
@@ -2329,6 +2713,30 @@
       </c>
       <c r="F55" s="9">
         <v>0</v>
+      </c>
+      <c r="I55" s="18" t="str">
+        <f>CONCATENATE(A61,A60,A59,A58,A57,A56,A55,A54)</f>
+        <v>11111111</v>
+      </c>
+      <c r="J55" s="18" t="str">
+        <f t="shared" ref="J55" si="62">CONCATENATE(B61,B60,B59,B58,B57,B56,B55,B54)</f>
+        <v>00000011</v>
+      </c>
+      <c r="K55" s="18" t="str">
+        <f t="shared" ref="K55" si="63">CONCATENATE(C61,C60,C59,C58,C57,C56,C55,C54)</f>
+        <v>00001000</v>
+      </c>
+      <c r="L55" s="18" t="str">
+        <f t="shared" ref="L55" si="64">CONCATENATE(D61,D60,D59,D58,D57,D56,D55,D54)</f>
+        <v>00100000</v>
+      </c>
+      <c r="M55" s="18" t="str">
+        <f t="shared" ref="M55" si="65">CONCATENATE(E61,E60,E59,E58,E57,E56,E55,E54)</f>
+        <v>11111111</v>
+      </c>
+      <c r="N55" s="18" t="str">
+        <f t="shared" ref="N55" si="66">CONCATENATE(F61,F60,F59,F58,F57,F56,F55,F54)</f>
+        <v>00000000</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.3">
@@ -2355,27 +2763,27 @@
         <v>11111111</v>
       </c>
       <c r="J56" s="5" t="str">
-        <f t="shared" ref="J56:O56" si="18">MID(J54,1,8)</f>
+        <f t="shared" ref="J56:O56" si="67">MID(J54,1,8)</f>
         <v>11000000</v>
       </c>
       <c r="K56" s="5" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="67"/>
         <v>00010000</v>
       </c>
       <c r="L56" s="5" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="67"/>
         <v>00000100</v>
       </c>
       <c r="M56" s="5" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="67"/>
         <v>11111111</v>
       </c>
       <c r="N56" s="5" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="67"/>
         <v>00000000</v>
       </c>
       <c r="O56" s="5" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="67"/>
         <v/>
       </c>
     </row>
@@ -2397,6 +2805,30 @@
       </c>
       <c r="F57" s="9">
         <v>0</v>
+      </c>
+      <c r="I57" s="18" t="str">
+        <f>MID(I55,1,8)</f>
+        <v>11111111</v>
+      </c>
+      <c r="J57" s="18" t="str">
+        <f t="shared" ref="J57:N57" si="68">MID(J55,1,8)</f>
+        <v>00000011</v>
+      </c>
+      <c r="K57" s="18" t="str">
+        <f t="shared" si="68"/>
+        <v>00001000</v>
+      </c>
+      <c r="L57" s="18" t="str">
+        <f t="shared" si="68"/>
+        <v>00100000</v>
+      </c>
+      <c r="M57" s="18" t="str">
+        <f t="shared" si="68"/>
+        <v>11111111</v>
+      </c>
+      <c r="N57" s="18" t="str">
+        <f t="shared" si="68"/>
+        <v>00000000</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.3">
@@ -2423,27 +2855,27 @@
         <v>FF</v>
       </c>
       <c r="J58" s="6" t="str">
-        <f t="shared" ref="J58:O58" si="19">BIN2HEX(J56,2)</f>
+        <f t="shared" ref="J58:O58" si="69">BIN2HEX(J56,2)</f>
         <v>C0</v>
       </c>
       <c r="K58" s="6" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="69"/>
         <v>10</v>
       </c>
       <c r="L58" s="6" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="69"/>
         <v>04</v>
       </c>
       <c r="M58" s="6" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="69"/>
         <v>FF</v>
       </c>
       <c r="N58" s="6" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="69"/>
         <v>00</v>
       </c>
       <c r="O58" s="6" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="69"/>
         <v>00</v>
       </c>
     </row>
@@ -2465,6 +2897,30 @@
       </c>
       <c r="F59" s="9">
         <v>0</v>
+      </c>
+      <c r="I59" s="21" t="str">
+        <f t="shared" ref="I59:N59" si="70">BIN2HEX(I57,2)</f>
+        <v>FF</v>
+      </c>
+      <c r="J59" s="21" t="str">
+        <f t="shared" si="70"/>
+        <v>03</v>
+      </c>
+      <c r="K59" s="21" t="str">
+        <f t="shared" si="70"/>
+        <v>08</v>
+      </c>
+      <c r="L59" s="21" t="str">
+        <f t="shared" si="70"/>
+        <v>20</v>
+      </c>
+      <c r="M59" s="21" t="str">
+        <f t="shared" si="70"/>
+        <v>FF</v>
+      </c>
+      <c r="N59" s="21" t="str">
+        <f t="shared" si="70"/>
+        <v>00</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.3">
@@ -2531,27 +2987,27 @@
         <v>11111111</v>
       </c>
       <c r="J65" t="str">
-        <f t="shared" ref="J65:O65" si="20">CONCATENATE(B65,B66,B67,B68,B69,B70,B71,B72)</f>
+        <f t="shared" ref="J65" si="71">CONCATENATE(B65,B66,B67,B68,B69,B70,B71,B72)</f>
         <v>10010000</v>
       </c>
       <c r="K65" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="K65" si="72">CONCATENATE(C65,C66,C67,C68,C69,C70,C71,C72)</f>
         <v>10010000</v>
       </c>
       <c r="L65" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="L65" si="73">CONCATENATE(D65,D66,D67,D68,D69,D70,D71,D72)</f>
         <v>10010000</v>
       </c>
       <c r="M65" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="M65" si="74">CONCATENATE(E65,E66,E67,E68,E69,E70,E71,E72)</f>
         <v>10000000</v>
       </c>
       <c r="N65" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="N65" si="75">CONCATENATE(F65,F66,F67,F68,F69,F70,F71,F72)</f>
         <v>00000000</v>
       </c>
       <c r="O65" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="O65" si="76">CONCATENATE(G65,G66,G67,G68,G69,G70,G71,G72)</f>
         <v/>
       </c>
     </row>
@@ -2573,6 +3029,30 @@
       </c>
       <c r="F66" s="3">
         <v>0</v>
+      </c>
+      <c r="I66" s="18" t="str">
+        <f>CONCATENATE(A72,A71,A70,A69,A68,A67,A66,A65)</f>
+        <v>11111111</v>
+      </c>
+      <c r="J66" s="18" t="str">
+        <f t="shared" ref="J66" si="77">CONCATENATE(B72,B71,B70,B69,B68,B67,B66,B65)</f>
+        <v>00001001</v>
+      </c>
+      <c r="K66" s="18" t="str">
+        <f t="shared" ref="K66" si="78">CONCATENATE(C72,C71,C70,C69,C68,C67,C66,C65)</f>
+        <v>00001001</v>
+      </c>
+      <c r="L66" s="18" t="str">
+        <f t="shared" ref="L66" si="79">CONCATENATE(D72,D71,D70,D69,D68,D67,D66,D65)</f>
+        <v>00001001</v>
+      </c>
+      <c r="M66" s="18" t="str">
+        <f t="shared" ref="M66" si="80">CONCATENATE(E72,E71,E70,E69,E68,E67,E66,E65)</f>
+        <v>00000001</v>
+      </c>
+      <c r="N66" s="18" t="str">
+        <f t="shared" ref="N66" si="81">CONCATENATE(F72,F71,F70,F69,F68,F67,F66,F65)</f>
+        <v>00000000</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.3">
@@ -2599,27 +3079,27 @@
         <v>11111111</v>
       </c>
       <c r="J67" s="5" t="str">
-        <f t="shared" ref="J67:O67" si="21">MID(J65,1,8)</f>
+        <f t="shared" ref="J67:O67" si="82">MID(J65,1,8)</f>
         <v>10010000</v>
       </c>
       <c r="K67" s="5" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="82"/>
         <v>10010000</v>
       </c>
       <c r="L67" s="5" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="82"/>
         <v>10010000</v>
       </c>
       <c r="M67" s="5" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="82"/>
         <v>10000000</v>
       </c>
       <c r="N67" s="5" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="82"/>
         <v>00000000</v>
       </c>
       <c r="O67" s="5" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="82"/>
         <v/>
       </c>
     </row>
@@ -2641,6 +3121,30 @@
       </c>
       <c r="F68" s="3">
         <v>0</v>
+      </c>
+      <c r="I68" s="18" t="str">
+        <f>MID(I66,1,8)</f>
+        <v>11111111</v>
+      </c>
+      <c r="J68" s="18" t="str">
+        <f t="shared" ref="J68:N68" si="83">MID(J66,1,8)</f>
+        <v>00001001</v>
+      </c>
+      <c r="K68" s="18" t="str">
+        <f t="shared" si="83"/>
+        <v>00001001</v>
+      </c>
+      <c r="L68" s="18" t="str">
+        <f t="shared" si="83"/>
+        <v>00001001</v>
+      </c>
+      <c r="M68" s="18" t="str">
+        <f t="shared" si="83"/>
+        <v>00000001</v>
+      </c>
+      <c r="N68" s="18" t="str">
+        <f t="shared" si="83"/>
+        <v>00000000</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.3">
@@ -2667,27 +3171,27 @@
         <v>FF</v>
       </c>
       <c r="J69" s="6" t="str">
-        <f t="shared" ref="J69:O69" si="22">BIN2HEX(J67,2)</f>
+        <f t="shared" ref="J69:O69" si="84">BIN2HEX(J67,2)</f>
         <v>90</v>
       </c>
       <c r="K69" s="6" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="84"/>
         <v>90</v>
       </c>
       <c r="L69" s="6" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="84"/>
         <v>90</v>
       </c>
       <c r="M69" s="6" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="84"/>
         <v>80</v>
       </c>
       <c r="N69" s="6" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="84"/>
         <v>00</v>
       </c>
       <c r="O69" s="6" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="84"/>
         <v>00</v>
       </c>
     </row>
@@ -2709,6 +3213,30 @@
       </c>
       <c r="F70" s="3">
         <v>0</v>
+      </c>
+      <c r="I70" s="21" t="str">
+        <f t="shared" ref="I70:N70" si="85">BIN2HEX(I68,2)</f>
+        <v>FF</v>
+      </c>
+      <c r="J70" s="21" t="str">
+        <f t="shared" si="85"/>
+        <v>09</v>
+      </c>
+      <c r="K70" s="21" t="str">
+        <f t="shared" si="85"/>
+        <v>09</v>
+      </c>
+      <c r="L70" s="21" t="str">
+        <f t="shared" si="85"/>
+        <v>09</v>
+      </c>
+      <c r="M70" s="21" t="str">
+        <f t="shared" si="85"/>
+        <v>01</v>
+      </c>
+      <c r="N70" s="21" t="str">
+        <f t="shared" si="85"/>
+        <v>00</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.3">
@@ -2775,27 +3303,27 @@
         <v>11111111</v>
       </c>
       <c r="J75" t="str">
-        <f t="shared" ref="J75:O75" si="23">CONCATENATE(B75,B76,B77,B78,B79,B80,B81,B82)</f>
+        <f t="shared" ref="J75" si="86">CONCATENATE(B75,B76,B77,B78,B79,B80,B81,B82)</f>
         <v>10010000</v>
       </c>
       <c r="K75" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" ref="K75" si="87">CONCATENATE(C75,C76,C77,C78,C79,C80,C81,C82)</f>
         <v>10010000</v>
       </c>
       <c r="L75" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" ref="L75" si="88">CONCATENATE(D75,D76,D77,D78,D79,D80,D81,D82)</f>
         <v>10010000</v>
       </c>
       <c r="M75" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" ref="M75" si="89">CONCATENATE(E75,E76,E77,E78,E79,E80,E81,E82)</f>
         <v>10000000</v>
       </c>
       <c r="N75" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" ref="N75" si="90">CONCATENATE(F75,F76,F77,F78,F79,F80,F81,F82)</f>
         <v>00000000</v>
       </c>
       <c r="O75" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" ref="O75" si="91">CONCATENATE(G75,G76,G77,G78,G79,G80,G81,G82)</f>
         <v/>
       </c>
     </row>
@@ -2817,6 +3345,30 @@
       </c>
       <c r="F76" s="3">
         <v>0</v>
+      </c>
+      <c r="I76" s="18" t="str">
+        <f>CONCATENATE(A82,A81,A80,A79,A78,A77,A76,A75)</f>
+        <v>11111111</v>
+      </c>
+      <c r="J76" s="18" t="str">
+        <f t="shared" ref="J76" si="92">CONCATENATE(B82,B81,B80,B79,B78,B77,B76,B75)</f>
+        <v>00001001</v>
+      </c>
+      <c r="K76" s="18" t="str">
+        <f t="shared" ref="K76" si="93">CONCATENATE(C82,C81,C80,C79,C78,C77,C76,C75)</f>
+        <v>00001001</v>
+      </c>
+      <c r="L76" s="18" t="str">
+        <f t="shared" ref="L76" si="94">CONCATENATE(D82,D81,D80,D79,D78,D77,D76,D75)</f>
+        <v>00001001</v>
+      </c>
+      <c r="M76" s="18" t="str">
+        <f t="shared" ref="M76" si="95">CONCATENATE(E82,E81,E80,E79,E78,E77,E76,E75)</f>
+        <v>00000001</v>
+      </c>
+      <c r="N76" s="18" t="str">
+        <f t="shared" ref="N76" si="96">CONCATENATE(F82,F81,F80,F79,F78,F77,F76,F75)</f>
+        <v>00000000</v>
       </c>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.3">
@@ -2843,27 +3395,27 @@
         <v>11111111</v>
       </c>
       <c r="J77" s="5" t="str">
-        <f t="shared" ref="J77:O77" si="24">MID(J75,1,8)</f>
+        <f t="shared" ref="J77:O77" si="97">MID(J75,1,8)</f>
         <v>10010000</v>
       </c>
       <c r="K77" s="5" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="97"/>
         <v>10010000</v>
       </c>
       <c r="L77" s="5" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="97"/>
         <v>10010000</v>
       </c>
       <c r="M77" s="5" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="97"/>
         <v>10000000</v>
       </c>
       <c r="N77" s="5" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="97"/>
         <v>00000000</v>
       </c>
       <c r="O77" s="5" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="97"/>
         <v/>
       </c>
     </row>
@@ -2885,6 +3437,30 @@
       </c>
       <c r="F78" s="3">
         <v>0</v>
+      </c>
+      <c r="I78" s="18" t="str">
+        <f>MID(I76,1,8)</f>
+        <v>11111111</v>
+      </c>
+      <c r="J78" s="18" t="str">
+        <f t="shared" ref="J78:N78" si="98">MID(J76,1,8)</f>
+        <v>00001001</v>
+      </c>
+      <c r="K78" s="18" t="str">
+        <f t="shared" si="98"/>
+        <v>00001001</v>
+      </c>
+      <c r="L78" s="18" t="str">
+        <f t="shared" si="98"/>
+        <v>00001001</v>
+      </c>
+      <c r="M78" s="18" t="str">
+        <f t="shared" si="98"/>
+        <v>00000001</v>
+      </c>
+      <c r="N78" s="18" t="str">
+        <f t="shared" si="98"/>
+        <v>00000000</v>
       </c>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.3">
@@ -2911,27 +3487,27 @@
         <v>FF</v>
       </c>
       <c r="J79" s="6" t="str">
-        <f t="shared" ref="J79:O79" si="25">BIN2HEX(J77,2)</f>
+        <f t="shared" ref="J79:O79" si="99">BIN2HEX(J77,2)</f>
         <v>90</v>
       </c>
       <c r="K79" s="6" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="99"/>
         <v>90</v>
       </c>
       <c r="L79" s="6" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="99"/>
         <v>90</v>
       </c>
       <c r="M79" s="6" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="99"/>
         <v>80</v>
       </c>
       <c r="N79" s="6" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="99"/>
         <v>00</v>
       </c>
       <c r="O79" s="6" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="99"/>
         <v>00</v>
       </c>
     </row>
@@ -2954,6 +3530,30 @@
       <c r="F80" s="3">
         <v>0</v>
       </c>
+      <c r="I80" s="21" t="str">
+        <f t="shared" ref="I80:N80" si="100">BIN2HEX(I78,2)</f>
+        <v>FF</v>
+      </c>
+      <c r="J80" s="21" t="str">
+        <f t="shared" si="100"/>
+        <v>09</v>
+      </c>
+      <c r="K80" s="21" t="str">
+        <f t="shared" si="100"/>
+        <v>09</v>
+      </c>
+      <c r="L80" s="21" t="str">
+        <f t="shared" si="100"/>
+        <v>09</v>
+      </c>
+      <c r="M80" s="21" t="str">
+        <f t="shared" si="100"/>
+        <v>01</v>
+      </c>
+      <c r="N80" s="21" t="str">
+        <f t="shared" si="100"/>
+        <v>00</v>
+      </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
@@ -2996,10 +3596,19 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="12">
+    <mergeCell ref="P6:T6"/>
+    <mergeCell ref="P4:T4"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="U6:V6"/>
     <mergeCell ref="P1:R1"/>
     <mergeCell ref="P3:R3"/>
     <mergeCell ref="P5:R5"/>
+    <mergeCell ref="P2:T2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3010,7 +3619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A9" sqref="A9:AN9"/>
     </sheetView>
   </sheetViews>
@@ -3130,48 +3739,48 @@
       <c r="AK8" s="10"/>
     </row>
     <row r="9" spans="1:40" ht="99" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="13"/>
-      <c r="R9" s="13"/>
-      <c r="S9" s="13"/>
-      <c r="T9" s="13"/>
-      <c r="U9" s="13"/>
-      <c r="V9" s="13"/>
-      <c r="W9" s="13"/>
-      <c r="X9" s="13"/>
-      <c r="Y9" s="13"/>
-      <c r="Z9" s="13"/>
-      <c r="AA9" s="13"/>
-      <c r="AB9" s="13"/>
-      <c r="AC9" s="13"/>
-      <c r="AD9" s="13"/>
-      <c r="AE9" s="13"/>
-      <c r="AF9" s="13"/>
-      <c r="AG9" s="13"/>
-      <c r="AH9" s="13"/>
-      <c r="AI9" s="13"/>
-      <c r="AJ9" s="13"/>
-      <c r="AK9" s="13"/>
-      <c r="AL9" s="13"/>
-      <c r="AM9" s="13"/>
-      <c r="AN9" s="13"/>
+      <c r="A9" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="16"/>
+      <c r="U9" s="16"/>
+      <c r="V9" s="16"/>
+      <c r="W9" s="16"/>
+      <c r="X9" s="16"/>
+      <c r="Y9" s="16"/>
+      <c r="Z9" s="16"/>
+      <c r="AA9" s="16"/>
+      <c r="AB9" s="16"/>
+      <c r="AC9" s="16"/>
+      <c r="AD9" s="16"/>
+      <c r="AE9" s="16"/>
+      <c r="AF9" s="16"/>
+      <c r="AG9" s="16"/>
+      <c r="AH9" s="16"/>
+      <c r="AI9" s="16"/>
+      <c r="AJ9" s="16"/>
+      <c r="AK9" s="16"/>
+      <c r="AL9" s="16"/>
+      <c r="AM9" s="16"/>
+      <c r="AN9" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Alphabet added in exel file
</commit_message>
<xml_diff>
--- a/led pattren1.xlsx
+++ b/led pattren1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SEPS e\dspic codes\pic_led_171019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SEPS e\dspic codes\pic_led_171019\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10824" tabRatio="550" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10824" tabRatio="550" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,6 +131,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -177,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -191,6 +197,16 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -203,16 +219,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,7 +504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F1:W21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
@@ -941,10 +950,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V82"/>
+  <dimension ref="A1:V137"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="I137" sqref="I137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -974,39 +983,39 @@
         <v>0</v>
       </c>
       <c r="G1" s="7"/>
-      <c r="I1" s="19" t="str">
+      <c r="I1" s="14" t="str">
         <f t="shared" ref="I1:N1" si="0">CONCATENATE(A1,A2,A3,A4,A5,A6,A7,A8)</f>
         <v>11111111</v>
       </c>
-      <c r="J1" s="19" t="str">
+      <c r="J1" s="14" t="str">
         <f t="shared" si="0"/>
         <v>10010000</v>
       </c>
-      <c r="K1" s="19" t="str">
+      <c r="K1" s="14" t="str">
         <f t="shared" si="0"/>
         <v>10010000</v>
       </c>
-      <c r="L1" s="19" t="str">
+      <c r="L1" s="14" t="str">
         <f t="shared" si="0"/>
         <v>10010000</v>
       </c>
-      <c r="M1" s="19" t="str">
+      <c r="M1" s="14" t="str">
         <f t="shared" si="0"/>
         <v>10000000</v>
       </c>
-      <c r="N1" s="19" t="str">
+      <c r="N1" s="14" t="str">
         <f t="shared" si="0"/>
         <v>00000000</v>
       </c>
-      <c r="O1" s="19" t="str">
+      <c r="O1" s="14" t="str">
         <f>CONCATENATE(G1,G2,G3,G4,G5,G6,G7,G8,G9,G10,G11,G12,G13,G14,G15,G16)</f>
         <v/>
       </c>
-      <c r="P1" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
+      <c r="P1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
       <c r="U1" s="17" t="s">
         <v>5</v>
       </c>
@@ -1032,31 +1041,31 @@
         <v>0</v>
       </c>
       <c r="G2" s="7"/>
-      <c r="I2" s="18" t="str">
+      <c r="I2" s="13" t="str">
         <f>CONCATENATE(A8,A7,A6,A5,A4,A3,A2,A1)</f>
         <v>11111111</v>
       </c>
-      <c r="J2" s="18" t="str">
+      <c r="J2" s="13" t="str">
         <f t="shared" ref="J2:N2" si="1">CONCATENATE(B8,B7,B6,B5,B4,B3,B2,B1)</f>
         <v>00001001</v>
       </c>
-      <c r="K2" s="18" t="str">
+      <c r="K2" s="13" t="str">
         <f t="shared" si="1"/>
         <v>00001001</v>
       </c>
-      <c r="L2" s="18" t="str">
+      <c r="L2" s="13" t="str">
         <f t="shared" si="1"/>
         <v>00001001</v>
       </c>
-      <c r="M2" s="18" t="str">
+      <c r="M2" s="13" t="str">
         <f t="shared" si="1"/>
         <v>00000001</v>
       </c>
-      <c r="N2" s="18" t="str">
+      <c r="N2" s="13" t="str">
         <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
-      <c r="O2" s="18"/>
+      <c r="O2" s="13"/>
       <c r="P2" s="17" t="s">
         <v>4</v>
       </c>
@@ -1090,7 +1099,7 @@
       </c>
       <c r="G3" s="7"/>
       <c r="I3" s="5" t="str">
-        <f t="shared" ref="I3:O4" si="2">MID(I1,1,8)</f>
+        <f t="shared" ref="I3:O3" si="2">MID(I1,1,8)</f>
         <v>11111111</v>
       </c>
       <c r="J3" s="5" t="str">
@@ -1117,11 +1126,11 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="P3" s="13" t="s">
+      <c r="P3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="19"/>
       <c r="U3" s="17" t="s">
         <v>5</v>
       </c>
@@ -1147,31 +1156,31 @@
         <v>0</v>
       </c>
       <c r="G4" s="7"/>
-      <c r="I4" s="18" t="str">
+      <c r="I4" s="13" t="str">
         <f>MID(I2,1,8)</f>
         <v>11111111</v>
       </c>
-      <c r="J4" s="18" t="str">
+      <c r="J4" s="13" t="str">
         <f t="shared" ref="J4:N4" si="3">MID(J2,1,8)</f>
         <v>00001001</v>
       </c>
-      <c r="K4" s="18" t="str">
+      <c r="K4" s="13" t="str">
         <f t="shared" si="3"/>
         <v>00001001</v>
       </c>
-      <c r="L4" s="18" t="str">
+      <c r="L4" s="13" t="str">
         <f t="shared" si="3"/>
         <v>00001001</v>
       </c>
-      <c r="M4" s="18" t="str">
+      <c r="M4" s="13" t="str">
         <f t="shared" si="3"/>
         <v>00000001</v>
       </c>
-      <c r="N4" s="18" t="str">
+      <c r="N4" s="13" t="str">
         <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
-      <c r="O4" s="18"/>
+      <c r="O4" s="13"/>
       <c r="P4" s="17" t="s">
         <v>4</v>
       </c>
@@ -1232,11 +1241,11 @@
         <f t="shared" si="4"/>
         <v>00</v>
       </c>
-      <c r="P5" s="14" t="s">
+      <c r="P5" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
       <c r="U5" s="17" t="s">
         <v>5</v>
       </c>
@@ -1262,31 +1271,31 @@
         <v>0</v>
       </c>
       <c r="G6" s="7"/>
-      <c r="I6" s="20" t="str">
+      <c r="I6" s="15" t="str">
         <f t="shared" si="4"/>
         <v>FF</v>
       </c>
-      <c r="J6" s="20" t="str">
+      <c r="J6" s="15" t="str">
         <f t="shared" si="4"/>
         <v>09</v>
       </c>
-      <c r="K6" s="20" t="str">
+      <c r="K6" s="15" t="str">
         <f t="shared" si="4"/>
         <v>09</v>
       </c>
-      <c r="L6" s="20" t="str">
+      <c r="L6" s="15" t="str">
         <f t="shared" si="4"/>
         <v>09</v>
       </c>
-      <c r="M6" s="20" t="str">
+      <c r="M6" s="15" t="str">
         <f t="shared" si="4"/>
         <v>01</v>
       </c>
-      <c r="N6" s="20" t="str">
+      <c r="N6" s="15" t="str">
         <f t="shared" si="4"/>
         <v>00</v>
       </c>
-      <c r="O6" s="20" t="str">
+      <c r="O6" s="15" t="str">
         <f t="shared" si="4"/>
         <v>00</v>
       </c>
@@ -1447,27 +1456,27 @@
         <v>0</v>
       </c>
       <c r="G13" s="8"/>
-      <c r="I13" s="18" t="str">
+      <c r="I13" s="13" t="str">
         <f>CONCATENATE(A19,A18,A17,A16,A15,A14,A13,A12)</f>
         <v>11111110</v>
       </c>
-      <c r="J13" s="18" t="str">
+      <c r="J13" s="13" t="str">
         <f t="shared" ref="J13:N13" si="6">CONCATENATE(B19,B18,B17,B16,B15,B14,B13,B12)</f>
         <v>00010001</v>
       </c>
-      <c r="K13" s="18" t="str">
+      <c r="K13" s="13" t="str">
         <f t="shared" si="6"/>
         <v>00010001</v>
       </c>
-      <c r="L13" s="18" t="str">
+      <c r="L13" s="13" t="str">
         <f t="shared" si="6"/>
         <v>00010001</v>
       </c>
-      <c r="M13" s="18" t="str">
+      <c r="M13" s="13" t="str">
         <f t="shared" si="6"/>
         <v>11111110</v>
       </c>
-      <c r="N13" s="18" t="str">
+      <c r="N13" s="13" t="str">
         <f t="shared" si="6"/>
         <v>00000000</v>
       </c>
@@ -1541,27 +1550,27 @@
         <v>0</v>
       </c>
       <c r="G15" s="8"/>
-      <c r="I15" s="18" t="str">
+      <c r="I15" s="13" t="str">
         <f>MID(I13,1,8)</f>
         <v>11111110</v>
       </c>
-      <c r="J15" s="18" t="str">
+      <c r="J15" s="13" t="str">
         <f t="shared" ref="J15:N15" si="8">MID(J13,1,8)</f>
         <v>00010001</v>
       </c>
-      <c r="K15" s="18" t="str">
+      <c r="K15" s="13" t="str">
         <f t="shared" si="8"/>
         <v>00010001</v>
       </c>
-      <c r="L15" s="18" t="str">
+      <c r="L15" s="13" t="str">
         <f t="shared" si="8"/>
         <v>00010001</v>
       </c>
-      <c r="M15" s="18" t="str">
+      <c r="M15" s="13" t="str">
         <f t="shared" si="8"/>
         <v>11111110</v>
       </c>
-      <c r="N15" s="18" t="str">
+      <c r="N15" s="13" t="str">
         <f t="shared" si="8"/>
         <v>00000000</v>
       </c>
@@ -1634,27 +1643,27 @@
       <c r="F17" s="3">
         <v>0</v>
       </c>
-      <c r="I17" s="21" t="str">
+      <c r="I17" s="16" t="str">
         <f t="shared" ref="I17:N17" si="10">BIN2HEX(I15,2)</f>
         <v>FE</v>
       </c>
-      <c r="J17" s="21" t="str">
+      <c r="J17" s="16" t="str">
         <f t="shared" si="10"/>
         <v>11</v>
       </c>
-      <c r="K17" s="21" t="str">
+      <c r="K17" s="16" t="str">
         <f t="shared" si="10"/>
         <v>11</v>
       </c>
-      <c r="L17" s="21" t="str">
+      <c r="L17" s="16" t="str">
         <f t="shared" si="10"/>
         <v>11</v>
       </c>
-      <c r="M17" s="21" t="str">
+      <c r="M17" s="16" t="str">
         <f t="shared" si="10"/>
         <v>FE</v>
       </c>
-      <c r="N17" s="21" t="str">
+      <c r="N17" s="16" t="str">
         <f t="shared" si="10"/>
         <v>00</v>
       </c>
@@ -1766,27 +1775,27 @@
       <c r="F24" s="3">
         <v>0</v>
       </c>
-      <c r="I24" s="18" t="str">
+      <c r="I24" s="13" t="str">
         <f>CONCATENATE(A30,A29,A28,A27,A26,A25,A24,A23)</f>
         <v>11111111</v>
       </c>
-      <c r="J24" s="18" t="str">
+      <c r="J24" s="13" t="str">
         <f t="shared" ref="J24" si="17">CONCATENATE(B30,B29,B28,B27,B26,B25,B24,B23)</f>
         <v>00011001</v>
       </c>
-      <c r="K24" s="18" t="str">
+      <c r="K24" s="13" t="str">
         <f t="shared" ref="K24" si="18">CONCATENATE(C30,C29,C28,C27,C26,C25,C24,C23)</f>
         <v>00111001</v>
       </c>
-      <c r="L24" s="18" t="str">
+      <c r="L24" s="13" t="str">
         <f t="shared" ref="L24" si="19">CONCATENATE(D30,D29,D28,D27,D26,D25,D24,D23)</f>
         <v>01011001</v>
       </c>
-      <c r="M24" s="18" t="str">
+      <c r="M24" s="13" t="str">
         <f t="shared" ref="M24" si="20">CONCATENATE(E30,E29,E28,E27,E26,E25,E24,E23)</f>
         <v>10011111</v>
       </c>
-      <c r="N24" s="18" t="str">
+      <c r="N24" s="13" t="str">
         <f t="shared" ref="N24" si="21">CONCATENATE(F30,F29,F28,F27,F26,F25,F24,F23)</f>
         <v>00000000</v>
       </c>
@@ -1858,27 +1867,27 @@
       <c r="F26" s="3">
         <v>0</v>
       </c>
-      <c r="I26" s="18" t="str">
+      <c r="I26" s="13" t="str">
         <f>MID(I24,1,8)</f>
         <v>11111111</v>
       </c>
-      <c r="J26" s="18" t="str">
+      <c r="J26" s="13" t="str">
         <f t="shared" ref="J26:N26" si="23">MID(J24,1,8)</f>
         <v>00011001</v>
       </c>
-      <c r="K26" s="18" t="str">
+      <c r="K26" s="13" t="str">
         <f t="shared" si="23"/>
         <v>00111001</v>
       </c>
-      <c r="L26" s="18" t="str">
+      <c r="L26" s="13" t="str">
         <f t="shared" si="23"/>
         <v>01011001</v>
       </c>
-      <c r="M26" s="18" t="str">
+      <c r="M26" s="13" t="str">
         <f t="shared" si="23"/>
         <v>10011111</v>
       </c>
-      <c r="N26" s="18" t="str">
+      <c r="N26" s="13" t="str">
         <f t="shared" si="23"/>
         <v>00000000</v>
       </c>
@@ -1950,27 +1959,27 @@
       <c r="F28" s="3">
         <v>0</v>
       </c>
-      <c r="I28" s="21" t="str">
+      <c r="I28" s="16" t="str">
         <f t="shared" ref="I28:N28" si="25">BIN2HEX(I26,2)</f>
         <v>FF</v>
       </c>
-      <c r="J28" s="21" t="str">
+      <c r="J28" s="16" t="str">
         <f t="shared" si="25"/>
         <v>19</v>
       </c>
-      <c r="K28" s="21" t="str">
+      <c r="K28" s="16" t="str">
         <f t="shared" si="25"/>
         <v>39</v>
       </c>
-      <c r="L28" s="21" t="str">
+      <c r="L28" s="16" t="str">
         <f t="shared" si="25"/>
         <v>59</v>
       </c>
-      <c r="M28" s="21" t="str">
+      <c r="M28" s="16" t="str">
         <f t="shared" si="25"/>
         <v>9F</v>
       </c>
-      <c r="N28" s="21" t="str">
+      <c r="N28" s="16" t="str">
         <f t="shared" si="25"/>
         <v>00</v>
       </c>
@@ -2082,27 +2091,27 @@
       <c r="F35" s="9">
         <v>0</v>
       </c>
-      <c r="I35" s="18" t="str">
+      <c r="I35" s="13" t="str">
         <f>CONCATENATE(A41,A40,A39,A38,A37,A36,A35,A34)</f>
         <v>11111111</v>
       </c>
-      <c r="J35" s="18" t="str">
+      <c r="J35" s="13" t="str">
         <f t="shared" ref="J35" si="32">CONCATENATE(B41,B40,B39,B38,B37,B36,B35,B34)</f>
         <v>00010000</v>
       </c>
-      <c r="K35" s="18" t="str">
+      <c r="K35" s="13" t="str">
         <f t="shared" ref="K35" si="33">CONCATENATE(C41,C40,C39,C38,C37,C36,C35,C34)</f>
         <v>00010000</v>
       </c>
-      <c r="L35" s="18" t="str">
+      <c r="L35" s="13" t="str">
         <f t="shared" ref="L35" si="34">CONCATENATE(D41,D40,D39,D38,D37,D36,D35,D34)</f>
         <v>00010000</v>
       </c>
-      <c r="M35" s="18" t="str">
+      <c r="M35" s="13" t="str">
         <f t="shared" ref="M35" si="35">CONCATENATE(E41,E40,E39,E38,E37,E36,E35,E34)</f>
         <v>11111111</v>
       </c>
-      <c r="N35" s="18" t="str">
+      <c r="N35" s="13" t="str">
         <f t="shared" ref="N35" si="36">CONCATENATE(F41,F40,F39,F38,F37,F36,F35,F34)</f>
         <v>00000000</v>
       </c>
@@ -2174,27 +2183,27 @@
       <c r="F37" s="9">
         <v>0</v>
       </c>
-      <c r="I37" s="18" t="str">
+      <c r="I37" s="13" t="str">
         <f>MID(I35,1,8)</f>
         <v>11111111</v>
       </c>
-      <c r="J37" s="18" t="str">
+      <c r="J37" s="13" t="str">
         <f t="shared" ref="J37:N37" si="38">MID(J35,1,8)</f>
         <v>00010000</v>
       </c>
-      <c r="K37" s="18" t="str">
+      <c r="K37" s="13" t="str">
         <f t="shared" si="38"/>
         <v>00010000</v>
       </c>
-      <c r="L37" s="18" t="str">
+      <c r="L37" s="13" t="str">
         <f t="shared" si="38"/>
         <v>00010000</v>
       </c>
-      <c r="M37" s="18" t="str">
+      <c r="M37" s="13" t="str">
         <f t="shared" si="38"/>
         <v>11111111</v>
       </c>
-      <c r="N37" s="18" t="str">
+      <c r="N37" s="13" t="str">
         <f t="shared" si="38"/>
         <v>00000000</v>
       </c>
@@ -2266,27 +2275,27 @@
       <c r="F39" s="9">
         <v>0</v>
       </c>
-      <c r="I39" s="21" t="str">
+      <c r="I39" s="16" t="str">
         <f t="shared" ref="I39:N39" si="40">BIN2HEX(I37,2)</f>
         <v>FF</v>
       </c>
-      <c r="J39" s="21" t="str">
+      <c r="J39" s="16" t="str">
         <f t="shared" si="40"/>
         <v>10</v>
       </c>
-      <c r="K39" s="21" t="str">
+      <c r="K39" s="16" t="str">
         <f t="shared" si="40"/>
         <v>10</v>
       </c>
-      <c r="L39" s="21" t="str">
+      <c r="L39" s="16" t="str">
         <f t="shared" si="40"/>
         <v>10</v>
       </c>
-      <c r="M39" s="21" t="str">
+      <c r="M39" s="16" t="str">
         <f t="shared" si="40"/>
         <v>FF</v>
       </c>
-      <c r="N39" s="21" t="str">
+      <c r="N39" s="16" t="str">
         <f t="shared" si="40"/>
         <v>00</v>
       </c>
@@ -2398,27 +2407,27 @@
       <c r="F45" s="9">
         <v>1</v>
       </c>
-      <c r="I45" s="18" t="str">
+      <c r="I45" s="13" t="str">
         <f>CONCATENATE(A51,A50,A49,A48,A47,A46,A45,A44)</f>
         <v>11111110</v>
       </c>
-      <c r="J45" s="18" t="str">
+      <c r="J45" s="13" t="str">
         <f t="shared" ref="J45" si="47">CONCATENATE(B51,B50,B49,B48,B47,B46,B45,B44)</f>
         <v>00010001</v>
       </c>
-      <c r="K45" s="18" t="str">
+      <c r="K45" s="13" t="str">
         <f t="shared" ref="K45" si="48">CONCATENATE(C51,C50,C49,C48,C47,C46,C45,C44)</f>
         <v>00010001</v>
       </c>
-      <c r="L45" s="18" t="str">
+      <c r="L45" s="13" t="str">
         <f t="shared" ref="L45" si="49">CONCATENATE(D51,D50,D49,D48,D47,D46,D45,D44)</f>
         <v>00010001</v>
       </c>
-      <c r="M45" s="18" t="str">
+      <c r="M45" s="13" t="str">
         <f t="shared" ref="M45" si="50">CONCATENATE(E51,E50,E49,E48,E47,E46,E45,E44)</f>
         <v>00010001</v>
       </c>
-      <c r="N45" s="18" t="str">
+      <c r="N45" s="13" t="str">
         <f t="shared" ref="N45" si="51">CONCATENATE(F51,F50,F49,F48,F47,F46,F45,F44)</f>
         <v>11111110</v>
       </c>
@@ -2490,27 +2499,27 @@
       <c r="F47" s="9">
         <v>1</v>
       </c>
-      <c r="I47" s="18" t="str">
+      <c r="I47" s="13" t="str">
         <f>MID(I45,1,8)</f>
         <v>11111110</v>
       </c>
-      <c r="J47" s="18" t="str">
+      <c r="J47" s="13" t="str">
         <f t="shared" ref="J47:N47" si="53">MID(J45,1,8)</f>
         <v>00010001</v>
       </c>
-      <c r="K47" s="18" t="str">
+      <c r="K47" s="13" t="str">
         <f t="shared" si="53"/>
         <v>00010001</v>
       </c>
-      <c r="L47" s="18" t="str">
+      <c r="L47" s="13" t="str">
         <f t="shared" si="53"/>
         <v>00010001</v>
       </c>
-      <c r="M47" s="18" t="str">
+      <c r="M47" s="13" t="str">
         <f t="shared" si="53"/>
         <v>00010001</v>
       </c>
-      <c r="N47" s="18" t="str">
+      <c r="N47" s="13" t="str">
         <f t="shared" si="53"/>
         <v>11111110</v>
       </c>
@@ -2582,27 +2591,27 @@
       <c r="F49" s="9">
         <v>1</v>
       </c>
-      <c r="I49" s="21" t="str">
+      <c r="I49" s="16" t="str">
         <f t="shared" ref="I49:N49" si="55">BIN2HEX(I47,2)</f>
         <v>FE</v>
       </c>
-      <c r="J49" s="21" t="str">
+      <c r="J49" s="16" t="str">
         <f t="shared" si="55"/>
         <v>11</v>
       </c>
-      <c r="K49" s="21" t="str">
+      <c r="K49" s="16" t="str">
         <f t="shared" si="55"/>
         <v>11</v>
       </c>
-      <c r="L49" s="21" t="str">
+      <c r="L49" s="16" t="str">
         <f t="shared" si="55"/>
         <v>11</v>
       </c>
-      <c r="M49" s="21" t="str">
+      <c r="M49" s="16" t="str">
         <f t="shared" si="55"/>
         <v>11</v>
       </c>
-      <c r="N49" s="21" t="str">
+      <c r="N49" s="16" t="str">
         <f t="shared" si="55"/>
         <v>FE</v>
       </c>
@@ -2714,27 +2723,27 @@
       <c r="F55" s="9">
         <v>0</v>
       </c>
-      <c r="I55" s="18" t="str">
+      <c r="I55" s="13" t="str">
         <f>CONCATENATE(A61,A60,A59,A58,A57,A56,A55,A54)</f>
         <v>11111111</v>
       </c>
-      <c r="J55" s="18" t="str">
+      <c r="J55" s="13" t="str">
         <f t="shared" ref="J55" si="62">CONCATENATE(B61,B60,B59,B58,B57,B56,B55,B54)</f>
         <v>00000011</v>
       </c>
-      <c r="K55" s="18" t="str">
+      <c r="K55" s="13" t="str">
         <f t="shared" ref="K55" si="63">CONCATENATE(C61,C60,C59,C58,C57,C56,C55,C54)</f>
         <v>00001000</v>
       </c>
-      <c r="L55" s="18" t="str">
+      <c r="L55" s="13" t="str">
         <f t="shared" ref="L55" si="64">CONCATENATE(D61,D60,D59,D58,D57,D56,D55,D54)</f>
         <v>00100000</v>
       </c>
-      <c r="M55" s="18" t="str">
+      <c r="M55" s="13" t="str">
         <f t="shared" ref="M55" si="65">CONCATENATE(E61,E60,E59,E58,E57,E56,E55,E54)</f>
         <v>11111111</v>
       </c>
-      <c r="N55" s="18" t="str">
+      <c r="N55" s="13" t="str">
         <f t="shared" ref="N55" si="66">CONCATENATE(F61,F60,F59,F58,F57,F56,F55,F54)</f>
         <v>00000000</v>
       </c>
@@ -2806,27 +2815,27 @@
       <c r="F57" s="9">
         <v>0</v>
       </c>
-      <c r="I57" s="18" t="str">
+      <c r="I57" s="13" t="str">
         <f>MID(I55,1,8)</f>
         <v>11111111</v>
       </c>
-      <c r="J57" s="18" t="str">
+      <c r="J57" s="13" t="str">
         <f t="shared" ref="J57:N57" si="68">MID(J55,1,8)</f>
         <v>00000011</v>
       </c>
-      <c r="K57" s="18" t="str">
+      <c r="K57" s="13" t="str">
         <f t="shared" si="68"/>
         <v>00001000</v>
       </c>
-      <c r="L57" s="18" t="str">
+      <c r="L57" s="13" t="str">
         <f t="shared" si="68"/>
         <v>00100000</v>
       </c>
-      <c r="M57" s="18" t="str">
+      <c r="M57" s="13" t="str">
         <f t="shared" si="68"/>
         <v>11111111</v>
       </c>
-      <c r="N57" s="18" t="str">
+      <c r="N57" s="13" t="str">
         <f t="shared" si="68"/>
         <v>00000000</v>
       </c>
@@ -2898,27 +2907,27 @@
       <c r="F59" s="9">
         <v>0</v>
       </c>
-      <c r="I59" s="21" t="str">
+      <c r="I59" s="16" t="str">
         <f t="shared" ref="I59:N59" si="70">BIN2HEX(I57,2)</f>
         <v>FF</v>
       </c>
-      <c r="J59" s="21" t="str">
+      <c r="J59" s="16" t="str">
         <f t="shared" si="70"/>
         <v>03</v>
       </c>
-      <c r="K59" s="21" t="str">
+      <c r="K59" s="16" t="str">
         <f t="shared" si="70"/>
         <v>08</v>
       </c>
-      <c r="L59" s="21" t="str">
+      <c r="L59" s="16" t="str">
         <f t="shared" si="70"/>
         <v>20</v>
       </c>
-      <c r="M59" s="21" t="str">
+      <c r="M59" s="16" t="str">
         <f t="shared" si="70"/>
         <v>FF</v>
       </c>
-      <c r="N59" s="21" t="str">
+      <c r="N59" s="16" t="str">
         <f t="shared" si="70"/>
         <v>00</v>
       </c>
@@ -2964,19 +2973,19 @@
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A65" s="2">
-        <v>1</v>
-      </c>
-      <c r="B65" s="2">
-        <v>1</v>
-      </c>
-      <c r="C65" s="2">
-        <v>1</v>
-      </c>
-      <c r="D65" s="2">
-        <v>1</v>
-      </c>
-      <c r="E65" s="2">
+      <c r="A65" s="23">
+        <v>1</v>
+      </c>
+      <c r="B65" s="23">
+        <v>1</v>
+      </c>
+      <c r="C65" s="23">
+        <v>1</v>
+      </c>
+      <c r="D65" s="23">
+        <v>1</v>
+      </c>
+      <c r="E65" s="23">
         <v>1</v>
       </c>
       <c r="F65" s="3">
@@ -2988,19 +2997,19 @@
       </c>
       <c r="J65" t="str">
         <f t="shared" ref="J65" si="71">CONCATENATE(B65,B66,B67,B68,B69,B70,B71,B72)</f>
-        <v>10010000</v>
+        <v>10011001</v>
       </c>
       <c r="K65" t="str">
         <f t="shared" ref="K65" si="72">CONCATENATE(C65,C66,C67,C68,C69,C70,C71,C72)</f>
-        <v>10010000</v>
+        <v>10011001</v>
       </c>
       <c r="L65" t="str">
         <f t="shared" ref="L65" si="73">CONCATENATE(D65,D66,D67,D68,D69,D70,D71,D72)</f>
-        <v>10010000</v>
+        <v>10011001</v>
       </c>
       <c r="M65" t="str">
         <f t="shared" ref="M65" si="74">CONCATENATE(E65,E66,E67,E68,E69,E70,E71,E72)</f>
-        <v>10000000</v>
+        <v>10000001</v>
       </c>
       <c r="N65" t="str">
         <f t="shared" ref="N65" si="75">CONCATENATE(F65,F66,F67,F68,F69,F70,F71,F72)</f>
@@ -3012,7 +3021,7 @@
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A66" s="2">
+      <c r="A66" s="23">
         <v>1</v>
       </c>
       <c r="B66" s="3">
@@ -3030,33 +3039,33 @@
       <c r="F66" s="3">
         <v>0</v>
       </c>
-      <c r="I66" s="18" t="str">
+      <c r="I66" s="13" t="str">
         <f>CONCATENATE(A72,A71,A70,A69,A68,A67,A66,A65)</f>
         <v>11111111</v>
       </c>
-      <c r="J66" s="18" t="str">
+      <c r="J66" s="13" t="str">
         <f t="shared" ref="J66" si="77">CONCATENATE(B72,B71,B70,B69,B68,B67,B66,B65)</f>
-        <v>00001001</v>
-      </c>
-      <c r="K66" s="18" t="str">
+        <v>10011001</v>
+      </c>
+      <c r="K66" s="13" t="str">
         <f t="shared" ref="K66" si="78">CONCATENATE(C72,C71,C70,C69,C68,C67,C66,C65)</f>
-        <v>00001001</v>
-      </c>
-      <c r="L66" s="18" t="str">
+        <v>10011001</v>
+      </c>
+      <c r="L66" s="13" t="str">
         <f t="shared" ref="L66" si="79">CONCATENATE(D72,D71,D70,D69,D68,D67,D66,D65)</f>
-        <v>00001001</v>
-      </c>
-      <c r="M66" s="18" t="str">
+        <v>10011001</v>
+      </c>
+      <c r="M66" s="13" t="str">
         <f t="shared" ref="M66" si="80">CONCATENATE(E72,E71,E70,E69,E68,E67,E66,E65)</f>
-        <v>00000001</v>
-      </c>
-      <c r="N66" s="18" t="str">
+        <v>10000001</v>
+      </c>
+      <c r="N66" s="13" t="str">
         <f t="shared" ref="N66" si="81">CONCATENATE(F72,F71,F70,F69,F68,F67,F66,F65)</f>
         <v>00000000</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A67" s="2">
+      <c r="A67" s="23">
         <v>1</v>
       </c>
       <c r="B67" s="3">
@@ -3080,19 +3089,19 @@
       </c>
       <c r="J67" s="5" t="str">
         <f t="shared" ref="J67:O67" si="82">MID(J65,1,8)</f>
-        <v>10010000</v>
+        <v>10011001</v>
       </c>
       <c r="K67" s="5" t="str">
         <f t="shared" si="82"/>
-        <v>10010000</v>
+        <v>10011001</v>
       </c>
       <c r="L67" s="5" t="str">
         <f t="shared" si="82"/>
-        <v>10010000</v>
+        <v>10011001</v>
       </c>
       <c r="M67" s="5" t="str">
         <f t="shared" si="82"/>
-        <v>10000000</v>
+        <v>10000001</v>
       </c>
       <c r="N67" s="5" t="str">
         <f t="shared" si="82"/>
@@ -3104,16 +3113,16 @@
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A68" s="2">
-        <v>1</v>
-      </c>
-      <c r="B68" s="2">
-        <v>1</v>
-      </c>
-      <c r="C68" s="2">
-        <v>1</v>
-      </c>
-      <c r="D68" s="2">
+      <c r="A68" s="23">
+        <v>1</v>
+      </c>
+      <c r="B68" s="23">
+        <v>1</v>
+      </c>
+      <c r="C68" s="23">
+        <v>1</v>
+      </c>
+      <c r="D68" s="23">
         <v>1</v>
       </c>
       <c r="E68" s="3">
@@ -3122,43 +3131,43 @@
       <c r="F68" s="3">
         <v>0</v>
       </c>
-      <c r="I68" s="18" t="str">
+      <c r="I68" s="13" t="str">
         <f>MID(I66,1,8)</f>
         <v>11111111</v>
       </c>
-      <c r="J68" s="18" t="str">
+      <c r="J68" s="13" t="str">
         <f t="shared" ref="J68:N68" si="83">MID(J66,1,8)</f>
-        <v>00001001</v>
-      </c>
-      <c r="K68" s="18" t="str">
+        <v>10011001</v>
+      </c>
+      <c r="K68" s="13" t="str">
         <f t="shared" si="83"/>
-        <v>00001001</v>
-      </c>
-      <c r="L68" s="18" t="str">
+        <v>10011001</v>
+      </c>
+      <c r="L68" s="13" t="str">
         <f t="shared" si="83"/>
-        <v>00001001</v>
-      </c>
-      <c r="M68" s="18" t="str">
+        <v>10011001</v>
+      </c>
+      <c r="M68" s="13" t="str">
         <f t="shared" si="83"/>
-        <v>00000001</v>
-      </c>
-      <c r="N68" s="18" t="str">
+        <v>10000001</v>
+      </c>
+      <c r="N68" s="13" t="str">
         <f t="shared" si="83"/>
         <v>00000000</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A69" s="2">
-        <v>1</v>
-      </c>
-      <c r="B69" s="3">
-        <v>0</v>
-      </c>
-      <c r="C69" s="3">
-        <v>0</v>
-      </c>
-      <c r="D69" s="3">
-        <v>0</v>
+      <c r="A69" s="23">
+        <v>1</v>
+      </c>
+      <c r="B69" s="23">
+        <v>1</v>
+      </c>
+      <c r="C69" s="23">
+        <v>1</v>
+      </c>
+      <c r="D69" s="23">
+        <v>1</v>
       </c>
       <c r="E69" s="3">
         <v>0</v>
@@ -3172,19 +3181,19 @@
       </c>
       <c r="J69" s="6" t="str">
         <f t="shared" ref="J69:O69" si="84">BIN2HEX(J67,2)</f>
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="K69" s="6" t="str">
         <f t="shared" si="84"/>
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="L69" s="6" t="str">
         <f t="shared" si="84"/>
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="M69" s="6" t="str">
         <f t="shared" si="84"/>
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="N69" s="6" t="str">
         <f t="shared" si="84"/>
@@ -3196,7 +3205,7 @@
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A70" s="2">
+      <c r="A70" s="23">
         <v>1</v>
       </c>
       <c r="B70" s="3">
@@ -3214,33 +3223,33 @@
       <c r="F70" s="3">
         <v>0</v>
       </c>
-      <c r="I70" s="21" t="str">
+      <c r="I70" s="16" t="str">
         <f t="shared" ref="I70:N70" si="85">BIN2HEX(I68,2)</f>
         <v>FF</v>
       </c>
-      <c r="J70" s="21" t="str">
+      <c r="J70" s="16" t="str">
         <f t="shared" si="85"/>
-        <v>09</v>
-      </c>
-      <c r="K70" s="21" t="str">
+        <v>99</v>
+      </c>
+      <c r="K70" s="16" t="str">
         <f t="shared" si="85"/>
-        <v>09</v>
-      </c>
-      <c r="L70" s="21" t="str">
+        <v>99</v>
+      </c>
+      <c r="L70" s="16" t="str">
         <f t="shared" si="85"/>
-        <v>09</v>
-      </c>
-      <c r="M70" s="21" t="str">
+        <v>99</v>
+      </c>
+      <c r="M70" s="16" t="str">
         <f t="shared" si="85"/>
-        <v>01</v>
-      </c>
-      <c r="N70" s="21" t="str">
+        <v>81</v>
+      </c>
+      <c r="N70" s="16" t="str">
         <f t="shared" si="85"/>
         <v>00</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A71" s="2">
+      <c r="A71" s="23">
         <v>1</v>
       </c>
       <c r="B71" s="3">
@@ -3260,67 +3269,67 @@
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A72" s="2">
-        <v>1</v>
-      </c>
-      <c r="B72" s="3">
-        <v>0</v>
-      </c>
-      <c r="C72" s="3">
-        <v>0</v>
-      </c>
-      <c r="D72" s="3">
-        <v>0</v>
-      </c>
-      <c r="E72" s="3">
-        <v>0</v>
+      <c r="A72" s="23">
+        <v>1</v>
+      </c>
+      <c r="B72" s="23">
+        <v>1</v>
+      </c>
+      <c r="C72" s="23">
+        <v>1</v>
+      </c>
+      <c r="D72" s="23">
+        <v>1</v>
+      </c>
+      <c r="E72" s="23">
+        <v>1</v>
       </c>
       <c r="F72" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A75" s="2">
-        <v>1</v>
-      </c>
-      <c r="B75" s="2">
-        <v>1</v>
-      </c>
-      <c r="C75" s="2">
-        <v>1</v>
-      </c>
-      <c r="D75" s="2">
-        <v>1</v>
-      </c>
-      <c r="E75" s="2">
-        <v>1</v>
-      </c>
-      <c r="F75" s="3">
-        <v>0</v>
+      <c r="A75" s="23">
+        <v>1</v>
+      </c>
+      <c r="B75" s="23">
+        <v>1</v>
+      </c>
+      <c r="C75" s="23">
+        <v>1</v>
+      </c>
+      <c r="D75" s="23">
+        <v>1</v>
+      </c>
+      <c r="E75" s="23">
+        <v>1</v>
+      </c>
+      <c r="F75" s="23">
+        <v>1</v>
       </c>
       <c r="I75" t="str">
         <f>CONCATENATE(A75,A76,A77,A78,A79,A80,A81,A82)</f>
-        <v>11111111</v>
+        <v>10000001</v>
       </c>
       <c r="J75" t="str">
         <f t="shared" ref="J75" si="86">CONCATENATE(B75,B76,B77,B78,B79,B80,B81,B82)</f>
-        <v>10010000</v>
+        <v>10000001</v>
       </c>
       <c r="K75" t="str">
         <f t="shared" ref="K75" si="87">CONCATENATE(C75,C76,C77,C78,C79,C80,C81,C82)</f>
-        <v>10010000</v>
+        <v>11111111</v>
       </c>
       <c r="L75" t="str">
         <f t="shared" ref="L75" si="88">CONCATENATE(D75,D76,D77,D78,D79,D80,D81,D82)</f>
-        <v>10010000</v>
+        <v>11111111</v>
       </c>
       <c r="M75" t="str">
         <f t="shared" ref="M75" si="89">CONCATENATE(E75,E76,E77,E78,E79,E80,E81,E82)</f>
-        <v>10000000</v>
+        <v>10000001</v>
       </c>
       <c r="N75" t="str">
         <f t="shared" ref="N75" si="90">CONCATENATE(F75,F76,F77,F78,F79,F80,F81,F82)</f>
-        <v>00000000</v>
+        <v>10000001</v>
       </c>
       <c r="O75" t="str">
         <f t="shared" ref="O75" si="91">CONCATENATE(G75,G76,G77,G78,G79,G80,G81,G82)</f>
@@ -3328,17 +3337,17 @@
       </c>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A76" s="2">
-        <v>1</v>
+      <c r="A76" s="3">
+        <v>0</v>
       </c>
       <c r="B76" s="3">
         <v>0</v>
       </c>
-      <c r="C76" s="3">
-        <v>0</v>
-      </c>
-      <c r="D76" s="3">
-        <v>0</v>
+      <c r="C76" s="23">
+        <v>1</v>
+      </c>
+      <c r="D76" s="23">
+        <v>1</v>
       </c>
       <c r="E76" s="3">
         <v>0</v>
@@ -3346,43 +3355,43 @@
       <c r="F76" s="3">
         <v>0</v>
       </c>
-      <c r="I76" s="18" t="str">
+      <c r="I76" s="13" t="str">
         <f>CONCATENATE(A82,A81,A80,A79,A78,A77,A76,A75)</f>
-        <v>11111111</v>
-      </c>
-      <c r="J76" s="18" t="str">
+        <v>10000001</v>
+      </c>
+      <c r="J76" s="13" t="str">
         <f t="shared" ref="J76" si="92">CONCATENATE(B82,B81,B80,B79,B78,B77,B76,B75)</f>
-        <v>00001001</v>
-      </c>
-      <c r="K76" s="18" t="str">
+        <v>10000001</v>
+      </c>
+      <c r="K76" s="13" t="str">
         <f t="shared" ref="K76" si="93">CONCATENATE(C82,C81,C80,C79,C78,C77,C76,C75)</f>
-        <v>00001001</v>
-      </c>
-      <c r="L76" s="18" t="str">
+        <v>11111111</v>
+      </c>
+      <c r="L76" s="13" t="str">
         <f t="shared" ref="L76" si="94">CONCATENATE(D82,D81,D80,D79,D78,D77,D76,D75)</f>
-        <v>00001001</v>
-      </c>
-      <c r="M76" s="18" t="str">
+        <v>11111111</v>
+      </c>
+      <c r="M76" s="13" t="str">
         <f t="shared" ref="M76" si="95">CONCATENATE(E82,E81,E80,E79,E78,E77,E76,E75)</f>
-        <v>00000001</v>
-      </c>
-      <c r="N76" s="18" t="str">
+        <v>10000001</v>
+      </c>
+      <c r="N76" s="13" t="str">
         <f t="shared" ref="N76" si="96">CONCATENATE(F82,F81,F80,F79,F78,F77,F76,F75)</f>
-        <v>00000000</v>
+        <v>10000001</v>
       </c>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A77" s="2">
-        <v>1</v>
+      <c r="A77" s="3">
+        <v>0</v>
       </c>
       <c r="B77" s="3">
         <v>0</v>
       </c>
-      <c r="C77" s="3">
-        <v>0</v>
-      </c>
-      <c r="D77" s="3">
-        <v>0</v>
+      <c r="C77" s="23">
+        <v>1</v>
+      </c>
+      <c r="D77" s="23">
+        <v>1</v>
       </c>
       <c r="E77" s="3">
         <v>0</v>
@@ -3392,27 +3401,27 @@
       </c>
       <c r="I77" s="5" t="str">
         <f>MID(I75,1,8)</f>
-        <v>11111111</v>
+        <v>10000001</v>
       </c>
       <c r="J77" s="5" t="str">
         <f t="shared" ref="J77:O77" si="97">MID(J75,1,8)</f>
-        <v>10010000</v>
+        <v>10000001</v>
       </c>
       <c r="K77" s="5" t="str">
         <f t="shared" si="97"/>
-        <v>10010000</v>
+        <v>11111111</v>
       </c>
       <c r="L77" s="5" t="str">
         <f t="shared" si="97"/>
-        <v>10010000</v>
+        <v>11111111</v>
       </c>
       <c r="M77" s="5" t="str">
         <f t="shared" si="97"/>
-        <v>10000000</v>
+        <v>10000001</v>
       </c>
       <c r="N77" s="5" t="str">
         <f t="shared" si="97"/>
-        <v>00000000</v>
+        <v>10000001</v>
       </c>
       <c r="O77" s="5" t="str">
         <f t="shared" si="97"/>
@@ -3420,16 +3429,16 @@
       </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A78" s="2">
-        <v>1</v>
-      </c>
-      <c r="B78" s="2">
-        <v>1</v>
-      </c>
-      <c r="C78" s="2">
-        <v>1</v>
-      </c>
-      <c r="D78" s="2">
+      <c r="A78" s="3">
+        <v>0</v>
+      </c>
+      <c r="B78" s="3">
+        <v>0</v>
+      </c>
+      <c r="C78" s="23">
+        <v>1</v>
+      </c>
+      <c r="D78" s="23">
         <v>1</v>
       </c>
       <c r="E78" s="3">
@@ -3438,43 +3447,43 @@
       <c r="F78" s="3">
         <v>0</v>
       </c>
-      <c r="I78" s="18" t="str">
+      <c r="I78" s="13" t="str">
         <f>MID(I76,1,8)</f>
-        <v>11111111</v>
-      </c>
-      <c r="J78" s="18" t="str">
+        <v>10000001</v>
+      </c>
+      <c r="J78" s="13" t="str">
         <f t="shared" ref="J78:N78" si="98">MID(J76,1,8)</f>
-        <v>00001001</v>
-      </c>
-      <c r="K78" s="18" t="str">
+        <v>10000001</v>
+      </c>
+      <c r="K78" s="13" t="str">
         <f t="shared" si="98"/>
-        <v>00001001</v>
-      </c>
-      <c r="L78" s="18" t="str">
+        <v>11111111</v>
+      </c>
+      <c r="L78" s="13" t="str">
         <f t="shared" si="98"/>
-        <v>00001001</v>
-      </c>
-      <c r="M78" s="18" t="str">
+        <v>11111111</v>
+      </c>
+      <c r="M78" s="13" t="str">
         <f t="shared" si="98"/>
-        <v>00000001</v>
-      </c>
-      <c r="N78" s="18" t="str">
+        <v>10000001</v>
+      </c>
+      <c r="N78" s="13" t="str">
         <f t="shared" si="98"/>
-        <v>00000000</v>
+        <v>10000001</v>
       </c>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A79" s="2">
-        <v>1</v>
+      <c r="A79" s="3">
+        <v>0</v>
       </c>
       <c r="B79" s="3">
         <v>0</v>
       </c>
-      <c r="C79" s="3">
-        <v>0</v>
-      </c>
-      <c r="D79" s="3">
-        <v>0</v>
+      <c r="C79" s="23">
+        <v>1</v>
+      </c>
+      <c r="D79" s="23">
+        <v>1</v>
       </c>
       <c r="E79" s="3">
         <v>0</v>
@@ -3484,27 +3493,27 @@
       </c>
       <c r="I79" s="6" t="str">
         <f>BIN2HEX(I77,2)</f>
-        <v>FF</v>
+        <v>81</v>
       </c>
       <c r="J79" s="6" t="str">
         <f t="shared" ref="J79:O79" si="99">BIN2HEX(J77,2)</f>
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="K79" s="6" t="str">
         <f t="shared" si="99"/>
-        <v>90</v>
+        <v>FF</v>
       </c>
       <c r="L79" s="6" t="str">
         <f t="shared" si="99"/>
-        <v>90</v>
+        <v>FF</v>
       </c>
       <c r="M79" s="6" t="str">
         <f t="shared" si="99"/>
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="N79" s="6" t="str">
         <f t="shared" si="99"/>
-        <v>00</v>
+        <v>81</v>
       </c>
       <c r="O79" s="6" t="str">
         <f t="shared" si="99"/>
@@ -3512,17 +3521,17 @@
       </c>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A80" s="2">
-        <v>1</v>
+      <c r="A80" s="3">
+        <v>0</v>
       </c>
       <c r="B80" s="3">
         <v>0</v>
       </c>
-      <c r="C80" s="3">
-        <v>0</v>
-      </c>
-      <c r="D80" s="3">
-        <v>0</v>
+      <c r="C80" s="23">
+        <v>1</v>
+      </c>
+      <c r="D80" s="23">
+        <v>1</v>
       </c>
       <c r="E80" s="3">
         <v>0</v>
@@ -3530,70 +3539,1664 @@
       <c r="F80" s="3">
         <v>0</v>
       </c>
-      <c r="I80" s="21" t="str">
+      <c r="I80" s="16" t="str">
         <f t="shared" ref="I80:N80" si="100">BIN2HEX(I78,2)</f>
+        <v>81</v>
+      </c>
+      <c r="J80" s="16" t="str">
+        <f t="shared" si="100"/>
+        <v>81</v>
+      </c>
+      <c r="K80" s="16" t="str">
+        <f t="shared" si="100"/>
         <v>FF</v>
       </c>
-      <c r="J80" s="21" t="str">
+      <c r="L80" s="16" t="str">
         <f t="shared" si="100"/>
-        <v>09</v>
-      </c>
-      <c r="K80" s="21" t="str">
+        <v>FF</v>
+      </c>
+      <c r="M80" s="16" t="str">
         <f t="shared" si="100"/>
-        <v>09</v>
-      </c>
-      <c r="L80" s="21" t="str">
+        <v>81</v>
+      </c>
+      <c r="N80" s="16" t="str">
         <f t="shared" si="100"/>
-        <v>09</v>
-      </c>
-      <c r="M80" s="21" t="str">
-        <f t="shared" si="100"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A81" s="3">
+        <v>0</v>
+      </c>
+      <c r="B81" s="3">
+        <v>0</v>
+      </c>
+      <c r="C81" s="23">
+        <v>1</v>
+      </c>
+      <c r="D81" s="23">
+        <v>1</v>
+      </c>
+      <c r="E81" s="3">
+        <v>0</v>
+      </c>
+      <c r="F81" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A82" s="23">
+        <v>1</v>
+      </c>
+      <c r="B82" s="23">
+        <v>1</v>
+      </c>
+      <c r="C82" s="23">
+        <v>1</v>
+      </c>
+      <c r="D82" s="23">
+        <v>1</v>
+      </c>
+      <c r="E82" s="23">
+        <v>1</v>
+      </c>
+      <c r="F82" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A85" s="23">
+        <v>1</v>
+      </c>
+      <c r="B85" s="23">
+        <v>1</v>
+      </c>
+      <c r="C85" s="23">
+        <v>1</v>
+      </c>
+      <c r="D85" s="23">
+        <v>1</v>
+      </c>
+      <c r="E85" s="3">
+        <v>0</v>
+      </c>
+      <c r="F85" s="3">
+        <v>0</v>
+      </c>
+      <c r="I85" t="str">
+        <f>CONCATENATE(A85,A86,A87,A88,A89,A90,A91,A92)</f>
+        <v>11111111</v>
+      </c>
+      <c r="J85" t="str">
+        <f t="shared" ref="J85" si="101">CONCATENATE(B85,B86,B87,B88,B89,B90,B91,B92)</f>
+        <v>10000001</v>
+      </c>
+      <c r="K85" t="str">
+        <f t="shared" ref="K85" si="102">CONCATENATE(C85,C86,C87,C88,C89,C90,C91,C92)</f>
+        <v>10000001</v>
+      </c>
+      <c r="L85" t="str">
+        <f t="shared" ref="L85" si="103">CONCATENATE(D85,D86,D87,D88,D89,D90,D91,D92)</f>
+        <v>10000001</v>
+      </c>
+      <c r="M85" t="str">
+        <f t="shared" ref="M85" si="104">CONCATENATE(E85,E86,E87,E88,E89,E90,E91,E92)</f>
+        <v>01111110</v>
+      </c>
+      <c r="N85" t="str">
+        <f t="shared" ref="N85" si="105">CONCATENATE(F85,F86,F87,F88,F89,F90,F91,F92)</f>
+        <v>00000000</v>
+      </c>
+      <c r="O85" t="str">
+        <f t="shared" ref="O85" si="106">CONCATENATE(G85,G86,G87,G88,G89,G90,G91,G92)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A86" s="23">
+        <v>1</v>
+      </c>
+      <c r="B86" s="3">
+        <v>0</v>
+      </c>
+      <c r="C86" s="3">
+        <v>0</v>
+      </c>
+      <c r="D86" s="3">
+        <v>0</v>
+      </c>
+      <c r="E86" s="24">
+        <v>1</v>
+      </c>
+      <c r="F86" s="3">
+        <v>0</v>
+      </c>
+      <c r="I86" s="13" t="str">
+        <f>CONCATENATE(A92,A91,A90,A89,A88,A87,A86,A85)</f>
+        <v>11111111</v>
+      </c>
+      <c r="J86" s="13" t="str">
+        <f t="shared" ref="J86" si="107">CONCATENATE(B92,B91,B90,B89,B88,B87,B86,B85)</f>
+        <v>10000001</v>
+      </c>
+      <c r="K86" s="13" t="str">
+        <f t="shared" ref="K86" si="108">CONCATENATE(C92,C91,C90,C89,C88,C87,C86,C85)</f>
+        <v>10000001</v>
+      </c>
+      <c r="L86" s="13" t="str">
+        <f t="shared" ref="L86" si="109">CONCATENATE(D92,D91,D90,D89,D88,D87,D86,D85)</f>
+        <v>10000001</v>
+      </c>
+      <c r="M86" s="13" t="str">
+        <f t="shared" ref="M86" si="110">CONCATENATE(E92,E91,E90,E89,E88,E87,E86,E85)</f>
+        <v>01111110</v>
+      </c>
+      <c r="N86" s="13" t="str">
+        <f t="shared" ref="N86" si="111">CONCATENATE(F92,F91,F90,F89,F88,F87,F86,F85)</f>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A87" s="23">
+        <v>1</v>
+      </c>
+      <c r="B87" s="3">
+        <v>0</v>
+      </c>
+      <c r="C87" s="3">
+        <v>0</v>
+      </c>
+      <c r="D87" s="3">
+        <v>0</v>
+      </c>
+      <c r="E87" s="23">
+        <v>1</v>
+      </c>
+      <c r="F87" s="3">
+        <v>0</v>
+      </c>
+      <c r="I87" s="5" t="str">
+        <f>MID(I85,1,8)</f>
+        <v>11111111</v>
+      </c>
+      <c r="J87" s="5" t="str">
+        <f t="shared" ref="J87:O87" si="112">MID(J85,1,8)</f>
+        <v>10000001</v>
+      </c>
+      <c r="K87" s="5" t="str">
+        <f t="shared" si="112"/>
+        <v>10000001</v>
+      </c>
+      <c r="L87" s="5" t="str">
+        <f t="shared" si="112"/>
+        <v>10000001</v>
+      </c>
+      <c r="M87" s="5" t="str">
+        <f t="shared" si="112"/>
+        <v>01111110</v>
+      </c>
+      <c r="N87" s="5" t="str">
+        <f t="shared" si="112"/>
+        <v>00000000</v>
+      </c>
+      <c r="O87" s="5" t="str">
+        <f t="shared" si="112"/>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A88" s="23">
+        <v>1</v>
+      </c>
+      <c r="B88" s="3">
+        <v>0</v>
+      </c>
+      <c r="C88" s="3">
+        <v>0</v>
+      </c>
+      <c r="D88" s="3">
+        <v>0</v>
+      </c>
+      <c r="E88" s="23">
+        <v>1</v>
+      </c>
+      <c r="F88" s="3">
+        <v>0</v>
+      </c>
+      <c r="I88" s="13" t="str">
+        <f>MID(I86,1,8)</f>
+        <v>11111111</v>
+      </c>
+      <c r="J88" s="13" t="str">
+        <f t="shared" ref="J88:N88" si="113">MID(J86,1,8)</f>
+        <v>10000001</v>
+      </c>
+      <c r="K88" s="13" t="str">
+        <f t="shared" si="113"/>
+        <v>10000001</v>
+      </c>
+      <c r="L88" s="13" t="str">
+        <f t="shared" si="113"/>
+        <v>10000001</v>
+      </c>
+      <c r="M88" s="13" t="str">
+        <f t="shared" si="113"/>
+        <v>01111110</v>
+      </c>
+      <c r="N88" s="13" t="str">
+        <f t="shared" si="113"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A89" s="23">
+        <v>1</v>
+      </c>
+      <c r="B89" s="3">
+        <v>0</v>
+      </c>
+      <c r="C89" s="3">
+        <v>0</v>
+      </c>
+      <c r="D89" s="3">
+        <v>0</v>
+      </c>
+      <c r="E89" s="23">
+        <v>1</v>
+      </c>
+      <c r="F89" s="3">
+        <v>0</v>
+      </c>
+      <c r="I89" s="6" t="str">
+        <f>BIN2HEX(I87,2)</f>
+        <v>FF</v>
+      </c>
+      <c r="J89" s="6" t="str">
+        <f t="shared" ref="J89:O89" si="114">BIN2HEX(J87,2)</f>
+        <v>81</v>
+      </c>
+      <c r="K89" s="6" t="str">
+        <f t="shared" si="114"/>
+        <v>81</v>
+      </c>
+      <c r="L89" s="6" t="str">
+        <f t="shared" si="114"/>
+        <v>81</v>
+      </c>
+      <c r="M89" s="6" t="str">
+        <f t="shared" si="114"/>
+        <v>7E</v>
+      </c>
+      <c r="N89" s="6" t="str">
+        <f t="shared" si="114"/>
+        <v>00</v>
+      </c>
+      <c r="O89" s="6" t="str">
+        <f t="shared" si="114"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A90" s="23">
+        <v>1</v>
+      </c>
+      <c r="B90" s="3">
+        <v>0</v>
+      </c>
+      <c r="C90" s="3">
+        <v>0</v>
+      </c>
+      <c r="D90" s="3">
+        <v>0</v>
+      </c>
+      <c r="E90" s="23">
+        <v>1</v>
+      </c>
+      <c r="F90" s="3">
+        <v>0</v>
+      </c>
+      <c r="I90" s="16" t="str">
+        <f t="shared" ref="I90:N90" si="115">BIN2HEX(I88,2)</f>
+        <v>FF</v>
+      </c>
+      <c r="J90" s="16" t="str">
+        <f t="shared" si="115"/>
+        <v>81</v>
+      </c>
+      <c r="K90" s="16" t="str">
+        <f t="shared" si="115"/>
+        <v>81</v>
+      </c>
+      <c r="L90" s="16" t="str">
+        <f t="shared" si="115"/>
+        <v>81</v>
+      </c>
+      <c r="M90" s="16" t="str">
+        <f t="shared" si="115"/>
+        <v>7E</v>
+      </c>
+      <c r="N90" s="16" t="str">
+        <f t="shared" si="115"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A91" s="23">
+        <v>1</v>
+      </c>
+      <c r="B91" s="3">
+        <v>0</v>
+      </c>
+      <c r="C91" s="3">
+        <v>0</v>
+      </c>
+      <c r="D91" s="3">
+        <v>0</v>
+      </c>
+      <c r="E91" s="23">
+        <v>1</v>
+      </c>
+      <c r="F91" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A92" s="23">
+        <v>1</v>
+      </c>
+      <c r="B92" s="23">
+        <v>1</v>
+      </c>
+      <c r="C92" s="23">
+        <v>1</v>
+      </c>
+      <c r="D92" s="23">
+        <v>1</v>
+      </c>
+      <c r="E92" s="3">
+        <v>0</v>
+      </c>
+      <c r="F92" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A95" s="9">
+        <v>1</v>
+      </c>
+      <c r="B95" s="3">
+        <v>0</v>
+      </c>
+      <c r="C95" s="3">
+        <v>0</v>
+      </c>
+      <c r="D95" s="3">
+        <v>0</v>
+      </c>
+      <c r="E95" s="25">
+        <v>1</v>
+      </c>
+      <c r="F95" s="3">
+        <v>0</v>
+      </c>
+      <c r="I95" t="str">
+        <f>CONCATENATE(A95,A96,A97,A98,A99,A100,A101,A102)</f>
+        <v>11111111</v>
+      </c>
+      <c r="J95" t="str">
+        <f t="shared" ref="J95" si="116">CONCATENATE(B95,B96,B97,B98,B99,B100,B101,B102)</f>
+        <v>01100000</v>
+      </c>
+      <c r="K95" t="str">
+        <f t="shared" ref="K95" si="117">CONCATENATE(C95,C96,C97,C98,C99,C100,C101,C102)</f>
+        <v>00010000</v>
+      </c>
+      <c r="L95" t="str">
+        <f t="shared" ref="L95" si="118">CONCATENATE(D95,D96,D97,D98,D99,D100,D101,D102)</f>
+        <v>01100100</v>
+      </c>
+      <c r="M95" t="str">
+        <f t="shared" ref="M95" si="119">CONCATENATE(E95,E96,E97,E98,E99,E100,E101,E102)</f>
+        <v>11111111</v>
+      </c>
+      <c r="N95" t="str">
+        <f t="shared" ref="N95" si="120">CONCATENATE(F95,F96,F97,F98,F99,F100,F101,F102)</f>
+        <v>00000000</v>
+      </c>
+      <c r="O95" t="str">
+        <f t="shared" ref="O95" si="121">CONCATENATE(G95,G96,G97,G98,G99,G100,G101,G102)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A96" s="9">
+        <v>1</v>
+      </c>
+      <c r="B96" s="9">
+        <v>1</v>
+      </c>
+      <c r="C96" s="3">
+        <v>0</v>
+      </c>
+      <c r="D96" s="25">
+        <v>1</v>
+      </c>
+      <c r="E96" s="25">
+        <v>1</v>
+      </c>
+      <c r="F96" s="3">
+        <v>0</v>
+      </c>
+      <c r="I96" s="13" t="str">
+        <f>CONCATENATE(A102,A101,A100,A99,A98,A97,A96,A95)</f>
+        <v>11111111</v>
+      </c>
+      <c r="J96" s="13" t="str">
+        <f t="shared" ref="J96" si="122">CONCATENATE(B102,B101,B100,B99,B98,B97,B96,B95)</f>
+        <v>00000110</v>
+      </c>
+      <c r="K96" s="13" t="str">
+        <f t="shared" ref="K96" si="123">CONCATENATE(C102,C101,C100,C99,C98,C97,C96,C95)</f>
+        <v>00001000</v>
+      </c>
+      <c r="L96" s="13" t="str">
+        <f t="shared" ref="L96" si="124">CONCATENATE(D102,D101,D100,D99,D98,D97,D96,D95)</f>
+        <v>00100110</v>
+      </c>
+      <c r="M96" s="13" t="str">
+        <f t="shared" ref="M96" si="125">CONCATENATE(E102,E101,E100,E99,E98,E97,E96,E95)</f>
+        <v>11111111</v>
+      </c>
+      <c r="N96" s="13" t="str">
+        <f t="shared" ref="N96" si="126">CONCATENATE(F102,F101,F100,F99,F98,F97,F96,F95)</f>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A97" s="9">
+        <v>1</v>
+      </c>
+      <c r="B97" s="9">
+        <v>1</v>
+      </c>
+      <c r="C97" s="3">
+        <v>0</v>
+      </c>
+      <c r="D97" s="25">
+        <v>1</v>
+      </c>
+      <c r="E97" s="25">
+        <v>1</v>
+      </c>
+      <c r="F97" s="3">
+        <v>0</v>
+      </c>
+      <c r="I97" s="5" t="str">
+        <f>MID(I95,1,8)</f>
+        <v>11111111</v>
+      </c>
+      <c r="J97" s="5" t="str">
+        <f t="shared" ref="J97:O97" si="127">MID(J95,1,8)</f>
+        <v>01100000</v>
+      </c>
+      <c r="K97" s="5" t="str">
+        <f t="shared" si="127"/>
+        <v>00010000</v>
+      </c>
+      <c r="L97" s="5" t="str">
+        <f t="shared" si="127"/>
+        <v>01100100</v>
+      </c>
+      <c r="M97" s="5" t="str">
+        <f t="shared" si="127"/>
+        <v>11111111</v>
+      </c>
+      <c r="N97" s="5" t="str">
+        <f t="shared" si="127"/>
+        <v>00000000</v>
+      </c>
+      <c r="O97" s="5" t="str">
+        <f t="shared" si="127"/>
+        <v/>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A98" s="9">
+        <v>1</v>
+      </c>
+      <c r="B98" s="3">
+        <v>0</v>
+      </c>
+      <c r="C98" s="9">
+        <v>1</v>
+      </c>
+      <c r="D98" s="3">
+        <v>0</v>
+      </c>
+      <c r="E98" s="25">
+        <v>1</v>
+      </c>
+      <c r="F98" s="3">
+        <v>0</v>
+      </c>
+      <c r="I98" s="13" t="str">
+        <f>MID(I96,1,8)</f>
+        <v>11111111</v>
+      </c>
+      <c r="J98" s="13" t="str">
+        <f t="shared" ref="J98:N98" si="128">MID(J96,1,8)</f>
+        <v>00000110</v>
+      </c>
+      <c r="K98" s="13" t="str">
+        <f t="shared" si="128"/>
+        <v>00001000</v>
+      </c>
+      <c r="L98" s="13" t="str">
+        <f t="shared" si="128"/>
+        <v>00100110</v>
+      </c>
+      <c r="M98" s="13" t="str">
+        <f t="shared" si="128"/>
+        <v>11111111</v>
+      </c>
+      <c r="N98" s="13" t="str">
+        <f t="shared" si="128"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A99" s="9">
+        <v>1</v>
+      </c>
+      <c r="B99" s="3">
+        <v>0</v>
+      </c>
+      <c r="C99" s="3">
+        <v>0</v>
+      </c>
+      <c r="D99" s="3">
+        <v>0</v>
+      </c>
+      <c r="E99" s="25">
+        <v>1</v>
+      </c>
+      <c r="F99" s="3">
+        <v>0</v>
+      </c>
+      <c r="I99" s="6" t="str">
+        <f>BIN2HEX(I97,2)</f>
+        <v>FF</v>
+      </c>
+      <c r="J99" s="6" t="str">
+        <f t="shared" ref="J99:O99" si="129">BIN2HEX(J97,2)</f>
+        <v>60</v>
+      </c>
+      <c r="K99" s="6" t="str">
+        <f t="shared" si="129"/>
+        <v>10</v>
+      </c>
+      <c r="L99" s="6" t="str">
+        <f t="shared" si="129"/>
+        <v>64</v>
+      </c>
+      <c r="M99" s="6" t="str">
+        <f t="shared" si="129"/>
+        <v>FF</v>
+      </c>
+      <c r="N99" s="6" t="str">
+        <f t="shared" si="129"/>
+        <v>00</v>
+      </c>
+      <c r="O99" s="6" t="str">
+        <f t="shared" si="129"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A100" s="9">
+        <v>1</v>
+      </c>
+      <c r="B100" s="3">
+        <v>0</v>
+      </c>
+      <c r="C100" s="3">
+        <v>0</v>
+      </c>
+      <c r="D100" s="3">
+        <v>1</v>
+      </c>
+      <c r="E100" s="25">
+        <v>1</v>
+      </c>
+      <c r="F100" s="3">
+        <v>0</v>
+      </c>
+      <c r="I100" s="16" t="str">
+        <f t="shared" ref="I100:N100" si="130">BIN2HEX(I98,2)</f>
+        <v>FF</v>
+      </c>
+      <c r="J100" s="16" t="str">
+        <f t="shared" si="130"/>
+        <v>06</v>
+      </c>
+      <c r="K100" s="16" t="str">
+        <f t="shared" si="130"/>
+        <v>08</v>
+      </c>
+      <c r="L100" s="16" t="str">
+        <f t="shared" si="130"/>
+        <v>26</v>
+      </c>
+      <c r="M100" s="16" t="str">
+        <f t="shared" si="130"/>
+        <v>FF</v>
+      </c>
+      <c r="N100" s="16" t="str">
+        <f t="shared" si="130"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A101" s="9">
+        <v>1</v>
+      </c>
+      <c r="B101" s="3">
+        <v>0</v>
+      </c>
+      <c r="C101" s="3">
+        <v>0</v>
+      </c>
+      <c r="D101" s="3">
+        <v>0</v>
+      </c>
+      <c r="E101" s="25">
+        <v>1</v>
+      </c>
+      <c r="F101" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A102" s="9">
+        <v>1</v>
+      </c>
+      <c r="B102" s="3">
+        <v>0</v>
+      </c>
+      <c r="C102" s="3">
+        <v>0</v>
+      </c>
+      <c r="D102" s="3">
+        <v>0</v>
+      </c>
+      <c r="E102" s="25">
+        <v>1</v>
+      </c>
+      <c r="F102" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="F103" s="12"/>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="F104" s="12"/>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A107" s="9">
+        <v>1</v>
+      </c>
+      <c r="B107" s="3">
+        <v>0</v>
+      </c>
+      <c r="C107" s="3">
+        <v>0</v>
+      </c>
+      <c r="D107" s="3">
+        <v>0</v>
+      </c>
+      <c r="E107" s="25">
+        <v>1</v>
+      </c>
+      <c r="F107" s="3">
+        <v>0</v>
+      </c>
+      <c r="I107" t="str">
+        <f>CONCATENATE(A107,A108,A109,A110,A111,A112,A113,A114)</f>
+        <v>11111111</v>
+      </c>
+      <c r="J107" t="str">
+        <f t="shared" ref="J107" si="131">CONCATENATE(B107,B108,B109,B110,B111,B112,B113,B114)</f>
+        <v>00000001</v>
+      </c>
+      <c r="K107" t="str">
+        <f t="shared" ref="K107" si="132">CONCATENATE(C107,C108,C109,C110,C111,C112,C113,C114)</f>
+        <v>00000001</v>
+      </c>
+      <c r="L107" t="str">
+        <f t="shared" ref="L107" si="133">CONCATENATE(D107,D108,D109,D110,D111,D112,D113,D114)</f>
+        <v>00000001</v>
+      </c>
+      <c r="M107" t="str">
+        <f t="shared" ref="M107" si="134">CONCATENATE(E107,E108,E109,E110,E111,E112,E113,E114)</f>
+        <v>11111111</v>
+      </c>
+      <c r="N107" t="str">
+        <f t="shared" ref="N107" si="135">CONCATENATE(F107,F108,F109,F110,F111,F112,F113,F114)</f>
+        <v>00000000</v>
+      </c>
+      <c r="O107" t="str">
+        <f t="shared" ref="O107" si="136">CONCATENATE(G107,G108,G109,G110,G111,G112,G113,G114)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A108" s="9">
+        <v>1</v>
+      </c>
+      <c r="B108" s="3">
+        <v>0</v>
+      </c>
+      <c r="C108" s="3">
+        <v>0</v>
+      </c>
+      <c r="D108" s="3">
+        <v>0</v>
+      </c>
+      <c r="E108" s="25">
+        <v>1</v>
+      </c>
+      <c r="F108" s="3">
+        <v>0</v>
+      </c>
+      <c r="I108" s="13" t="str">
+        <f>CONCATENATE(A114,A113,A112,A111,A110,A109,A108,A107)</f>
+        <v>11111111</v>
+      </c>
+      <c r="J108" s="13" t="str">
+        <f t="shared" ref="J108" si="137">CONCATENATE(B114,B113,B112,B111,B110,B109,B108,B107)</f>
+        <v>10000000</v>
+      </c>
+      <c r="K108" s="13" t="str">
+        <f t="shared" ref="K108" si="138">CONCATENATE(C114,C113,C112,C111,C110,C109,C108,C107)</f>
+        <v>10000000</v>
+      </c>
+      <c r="L108" s="13" t="str">
+        <f t="shared" ref="L108" si="139">CONCATENATE(D114,D113,D112,D111,D110,D109,D108,D107)</f>
+        <v>10000000</v>
+      </c>
+      <c r="M108" s="13" t="str">
+        <f t="shared" ref="M108" si="140">CONCATENATE(E114,E113,E112,E111,E110,E109,E108,E107)</f>
+        <v>11111111</v>
+      </c>
+      <c r="N108" s="13" t="str">
+        <f t="shared" ref="N108" si="141">CONCATENATE(F114,F113,F112,F111,F110,F109,F108,F107)</f>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A109" s="9">
+        <v>1</v>
+      </c>
+      <c r="B109" s="3">
+        <v>0</v>
+      </c>
+      <c r="C109" s="3">
+        <v>0</v>
+      </c>
+      <c r="D109" s="3">
+        <v>0</v>
+      </c>
+      <c r="E109" s="25">
+        <v>1</v>
+      </c>
+      <c r="F109" s="3">
+        <v>0</v>
+      </c>
+      <c r="I109" s="5" t="str">
+        <f>MID(I107,1,8)</f>
+        <v>11111111</v>
+      </c>
+      <c r="J109" s="5" t="str">
+        <f t="shared" ref="J109:O109" si="142">MID(J107,1,8)</f>
+        <v>00000001</v>
+      </c>
+      <c r="K109" s="5" t="str">
+        <f t="shared" si="142"/>
+        <v>00000001</v>
+      </c>
+      <c r="L109" s="5" t="str">
+        <f t="shared" si="142"/>
+        <v>00000001</v>
+      </c>
+      <c r="M109" s="5" t="str">
+        <f t="shared" si="142"/>
+        <v>11111111</v>
+      </c>
+      <c r="N109" s="5" t="str">
+        <f t="shared" si="142"/>
+        <v>00000000</v>
+      </c>
+      <c r="O109" s="5" t="str">
+        <f t="shared" si="142"/>
+        <v/>
+      </c>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A110" s="9">
+        <v>1</v>
+      </c>
+      <c r="B110" s="3">
+        <v>0</v>
+      </c>
+      <c r="C110" s="3">
+        <v>0</v>
+      </c>
+      <c r="D110" s="3">
+        <v>0</v>
+      </c>
+      <c r="E110" s="25">
+        <v>1</v>
+      </c>
+      <c r="F110" s="3">
+        <v>0</v>
+      </c>
+      <c r="I110" s="13" t="str">
+        <f>MID(I108,1,8)</f>
+        <v>11111111</v>
+      </c>
+      <c r="J110" s="13" t="str">
+        <f t="shared" ref="J110:N110" si="143">MID(J108,1,8)</f>
+        <v>10000000</v>
+      </c>
+      <c r="K110" s="13" t="str">
+        <f t="shared" si="143"/>
+        <v>10000000</v>
+      </c>
+      <c r="L110" s="13" t="str">
+        <f t="shared" si="143"/>
+        <v>10000000</v>
+      </c>
+      <c r="M110" s="13" t="str">
+        <f t="shared" si="143"/>
+        <v>11111111</v>
+      </c>
+      <c r="N110" s="13" t="str">
+        <f t="shared" si="143"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A111" s="9">
+        <v>1</v>
+      </c>
+      <c r="B111" s="3">
+        <v>0</v>
+      </c>
+      <c r="C111" s="3">
+        <v>0</v>
+      </c>
+      <c r="D111" s="3">
+        <v>0</v>
+      </c>
+      <c r="E111" s="25">
+        <v>1</v>
+      </c>
+      <c r="F111" s="3">
+        <v>0</v>
+      </c>
+      <c r="I111" s="6" t="str">
+        <f>BIN2HEX(I109,2)</f>
+        <v>FF</v>
+      </c>
+      <c r="J111" s="6" t="str">
+        <f t="shared" ref="J111:O111" si="144">BIN2HEX(J109,2)</f>
         <v>01</v>
       </c>
-      <c r="N80" s="21" t="str">
-        <f t="shared" si="100"/>
+      <c r="K111" s="6" t="str">
+        <f t="shared" si="144"/>
+        <v>01</v>
+      </c>
+      <c r="L111" s="6" t="str">
+        <f t="shared" si="144"/>
+        <v>01</v>
+      </c>
+      <c r="M111" s="6" t="str">
+        <f t="shared" si="144"/>
+        <v>FF</v>
+      </c>
+      <c r="N111" s="6" t="str">
+        <f t="shared" si="144"/>
         <v>00</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" s="2">
-        <v>1</v>
-      </c>
-      <c r="B81" s="3">
-        <v>0</v>
-      </c>
-      <c r="C81" s="3">
-        <v>0</v>
-      </c>
-      <c r="D81" s="3">
-        <v>0</v>
-      </c>
-      <c r="E81" s="3">
-        <v>0</v>
-      </c>
-      <c r="F81" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" s="2">
-        <v>1</v>
-      </c>
-      <c r="B82" s="3">
-        <v>0</v>
-      </c>
-      <c r="C82" s="3">
-        <v>0</v>
-      </c>
-      <c r="D82" s="3">
-        <v>0</v>
-      </c>
-      <c r="E82" s="3">
-        <v>0</v>
-      </c>
-      <c r="F82" s="3">
-        <v>0</v>
-      </c>
+      <c r="O111" s="6" t="str">
+        <f t="shared" si="144"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A112" s="9">
+        <v>1</v>
+      </c>
+      <c r="B112" s="3">
+        <v>0</v>
+      </c>
+      <c r="C112" s="3">
+        <v>0</v>
+      </c>
+      <c r="D112" s="3">
+        <v>0</v>
+      </c>
+      <c r="E112" s="25">
+        <v>1</v>
+      </c>
+      <c r="F112" s="3">
+        <v>0</v>
+      </c>
+      <c r="I112" s="16" t="str">
+        <f t="shared" ref="I112:N112" si="145">BIN2HEX(I110,2)</f>
+        <v>FF</v>
+      </c>
+      <c r="J112" s="16" t="str">
+        <f t="shared" si="145"/>
+        <v>80</v>
+      </c>
+      <c r="K112" s="16" t="str">
+        <f t="shared" si="145"/>
+        <v>80</v>
+      </c>
+      <c r="L112" s="16" t="str">
+        <f t="shared" si="145"/>
+        <v>80</v>
+      </c>
+      <c r="M112" s="16" t="str">
+        <f t="shared" si="145"/>
+        <v>FF</v>
+      </c>
+      <c r="N112" s="16" t="str">
+        <f t="shared" si="145"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A113" s="9">
+        <v>1</v>
+      </c>
+      <c r="B113" s="3">
+        <v>0</v>
+      </c>
+      <c r="C113" s="3">
+        <v>0</v>
+      </c>
+      <c r="D113" s="3">
+        <v>0</v>
+      </c>
+      <c r="E113" s="25">
+        <v>1</v>
+      </c>
+      <c r="F113" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A114" s="9">
+        <v>1</v>
+      </c>
+      <c r="B114" s="25">
+        <v>1</v>
+      </c>
+      <c r="C114" s="25">
+        <v>1</v>
+      </c>
+      <c r="D114" s="25">
+        <v>1</v>
+      </c>
+      <c r="E114" s="25">
+        <v>1</v>
+      </c>
+      <c r="F114" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A119" s="9">
+        <v>1</v>
+      </c>
+      <c r="B119" s="3">
+        <v>0</v>
+      </c>
+      <c r="C119" s="3">
+        <v>0</v>
+      </c>
+      <c r="D119" s="3">
+        <v>0</v>
+      </c>
+      <c r="E119" s="25">
+        <v>1</v>
+      </c>
+      <c r="F119" s="3">
+        <v>0</v>
+      </c>
+      <c r="I119" t="str">
+        <f>CONCATENATE(A119,A120,A121,A122,A123,A124,A125,A126)</f>
+        <v>11111111</v>
+      </c>
+      <c r="J119" t="str">
+        <f t="shared" ref="J119" si="146">CONCATENATE(B119,B120,B121,B122,B123,B124,B125,B126)</f>
+        <v>00011000</v>
+      </c>
+      <c r="K119" t="str">
+        <f t="shared" ref="K119" si="147">CONCATENATE(C119,C120,C121,C122,C123,C124,C125,C126)</f>
+        <v>00100100</v>
+      </c>
+      <c r="L119" t="str">
+        <f t="shared" ref="L119" si="148">CONCATENATE(D119,D120,D121,D122,D123,D124,D125,D126)</f>
+        <v>01000010</v>
+      </c>
+      <c r="M119" t="str">
+        <f t="shared" ref="M119" si="149">CONCATENATE(E119,E120,E121,E122,E123,E124,E125,E126)</f>
+        <v>10000001</v>
+      </c>
+      <c r="N119" t="str">
+        <f t="shared" ref="N119" si="150">CONCATENATE(F119,F120,F121,F122,F123,F124,F125,F126)</f>
+        <v>00000000</v>
+      </c>
+      <c r="O119" t="str">
+        <f t="shared" ref="O119" si="151">CONCATENATE(G119,G120,G121,G122,G123,G124,G125,G126)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="120" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A120" s="9">
+        <v>1</v>
+      </c>
+      <c r="B120" s="3">
+        <v>0</v>
+      </c>
+      <c r="C120" s="3">
+        <v>0</v>
+      </c>
+      <c r="D120" s="25">
+        <v>1</v>
+      </c>
+      <c r="E120" s="3">
+        <v>0</v>
+      </c>
+      <c r="F120" s="3">
+        <v>0</v>
+      </c>
+      <c r="I120" s="13" t="str">
+        <f>CONCATENATE(A126,A125,A124,A123,A122,A121,A120,A119)</f>
+        <v>11111111</v>
+      </c>
+      <c r="J120" s="13" t="str">
+        <f t="shared" ref="J120" si="152">CONCATENATE(B126,B125,B124,B123,B122,B121,B120,B119)</f>
+        <v>00011000</v>
+      </c>
+      <c r="K120" s="13" t="str">
+        <f t="shared" ref="K120" si="153">CONCATENATE(C126,C125,C124,C123,C122,C121,C120,C119)</f>
+        <v>00100100</v>
+      </c>
+      <c r="L120" s="13" t="str">
+        <f t="shared" ref="L120" si="154">CONCATENATE(D126,D125,D124,D123,D122,D121,D120,D119)</f>
+        <v>01000010</v>
+      </c>
+      <c r="M120" s="13" t="str">
+        <f t="shared" ref="M120" si="155">CONCATENATE(E126,E125,E124,E123,E122,E121,E120,E119)</f>
+        <v>10000001</v>
+      </c>
+      <c r="N120" s="13" t="str">
+        <f t="shared" ref="N120" si="156">CONCATENATE(F126,F125,F124,F123,F122,F121,F120,F119)</f>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="121" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A121" s="9">
+        <v>1</v>
+      </c>
+      <c r="B121" s="3">
+        <v>0</v>
+      </c>
+      <c r="C121" s="25">
+        <v>1</v>
+      </c>
+      <c r="D121" s="3">
+        <v>0</v>
+      </c>
+      <c r="E121" s="3">
+        <v>0</v>
+      </c>
+      <c r="F121" s="3">
+        <v>0</v>
+      </c>
+      <c r="I121" s="5" t="str">
+        <f>MID(I119,1,8)</f>
+        <v>11111111</v>
+      </c>
+      <c r="J121" s="5" t="str">
+        <f t="shared" ref="J121:O121" si="157">MID(J119,1,8)</f>
+        <v>00011000</v>
+      </c>
+      <c r="K121" s="5" t="str">
+        <f t="shared" si="157"/>
+        <v>00100100</v>
+      </c>
+      <c r="L121" s="5" t="str">
+        <f t="shared" si="157"/>
+        <v>01000010</v>
+      </c>
+      <c r="M121" s="5" t="str">
+        <f t="shared" si="157"/>
+        <v>10000001</v>
+      </c>
+      <c r="N121" s="5" t="str">
+        <f t="shared" si="157"/>
+        <v>00000000</v>
+      </c>
+      <c r="O121" s="5" t="str">
+        <f t="shared" si="157"/>
+        <v/>
+      </c>
+    </row>
+    <row r="122" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A122" s="9">
+        <v>1</v>
+      </c>
+      <c r="B122" s="25">
+        <v>1</v>
+      </c>
+      <c r="C122" s="3">
+        <v>0</v>
+      </c>
+      <c r="D122" s="3">
+        <v>0</v>
+      </c>
+      <c r="E122" s="3">
+        <v>0</v>
+      </c>
+      <c r="F122" s="3">
+        <v>0</v>
+      </c>
+      <c r="I122" s="13" t="str">
+        <f>MID(I120,1,8)</f>
+        <v>11111111</v>
+      </c>
+      <c r="J122" s="13" t="str">
+        <f t="shared" ref="J122:N122" si="158">MID(J120,1,8)</f>
+        <v>00011000</v>
+      </c>
+      <c r="K122" s="13" t="str">
+        <f t="shared" si="158"/>
+        <v>00100100</v>
+      </c>
+      <c r="L122" s="13" t="str">
+        <f t="shared" si="158"/>
+        <v>01000010</v>
+      </c>
+      <c r="M122" s="13" t="str">
+        <f t="shared" si="158"/>
+        <v>10000001</v>
+      </c>
+      <c r="N122" s="13" t="str">
+        <f t="shared" si="158"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A123" s="9">
+        <v>1</v>
+      </c>
+      <c r="B123" s="25">
+        <v>1</v>
+      </c>
+      <c r="C123" s="3">
+        <v>0</v>
+      </c>
+      <c r="D123" s="3">
+        <v>0</v>
+      </c>
+      <c r="E123" s="3">
+        <v>0</v>
+      </c>
+      <c r="F123" s="3">
+        <v>0</v>
+      </c>
+      <c r="I123" s="6" t="str">
+        <f>BIN2HEX(I121,2)</f>
+        <v>FF</v>
+      </c>
+      <c r="J123" s="6" t="str">
+        <f t="shared" ref="J123:O123" si="159">BIN2HEX(J121,2)</f>
+        <v>18</v>
+      </c>
+      <c r="K123" s="6" t="str">
+        <f t="shared" si="159"/>
+        <v>24</v>
+      </c>
+      <c r="L123" s="6" t="str">
+        <f t="shared" si="159"/>
+        <v>42</v>
+      </c>
+      <c r="M123" s="6" t="str">
+        <f t="shared" si="159"/>
+        <v>81</v>
+      </c>
+      <c r="N123" s="6" t="str">
+        <f t="shared" si="159"/>
+        <v>00</v>
+      </c>
+      <c r="O123" s="6" t="str">
+        <f t="shared" si="159"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="124" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A124" s="9">
+        <v>1</v>
+      </c>
+      <c r="B124" s="3">
+        <v>0</v>
+      </c>
+      <c r="C124" s="25">
+        <v>1</v>
+      </c>
+      <c r="D124" s="3">
+        <v>0</v>
+      </c>
+      <c r="E124" s="3">
+        <v>0</v>
+      </c>
+      <c r="F124" s="3">
+        <v>0</v>
+      </c>
+      <c r="I124" s="16" t="str">
+        <f t="shared" ref="I124:N124" si="160">BIN2HEX(I122,2)</f>
+        <v>FF</v>
+      </c>
+      <c r="J124" s="16" t="str">
+        <f t="shared" si="160"/>
+        <v>18</v>
+      </c>
+      <c r="K124" s="16" t="str">
+        <f t="shared" si="160"/>
+        <v>24</v>
+      </c>
+      <c r="L124" s="16" t="str">
+        <f t="shared" si="160"/>
+        <v>42</v>
+      </c>
+      <c r="M124" s="16" t="str">
+        <f t="shared" si="160"/>
+        <v>81</v>
+      </c>
+      <c r="N124" s="16" t="str">
+        <f t="shared" si="160"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="125" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A125" s="9">
+        <v>1</v>
+      </c>
+      <c r="B125" s="3">
+        <v>0</v>
+      </c>
+      <c r="C125" s="3">
+        <v>0</v>
+      </c>
+      <c r="D125" s="25">
+        <v>1</v>
+      </c>
+      <c r="E125" s="3">
+        <v>0</v>
+      </c>
+      <c r="F125" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A126" s="9">
+        <v>1</v>
+      </c>
+      <c r="B126" s="3">
+        <v>0</v>
+      </c>
+      <c r="C126" s="3">
+        <v>0</v>
+      </c>
+      <c r="D126" s="3">
+        <v>0</v>
+      </c>
+      <c r="E126" s="25">
+        <v>1</v>
+      </c>
+      <c r="F126" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A129" s="23">
+        <v>1</v>
+      </c>
+      <c r="B129" s="23">
+        <v>1</v>
+      </c>
+      <c r="C129" s="23">
+        <v>1</v>
+      </c>
+      <c r="D129" s="23">
+        <v>1</v>
+      </c>
+      <c r="E129" s="3">
+        <v>0</v>
+      </c>
+      <c r="F129" s="3">
+        <v>0</v>
+      </c>
+      <c r="I129" t="str">
+        <f>CONCATENATE(A129,A130,A131,A132,A133,A134,A135,A136)</f>
+        <v>11111111</v>
+      </c>
+      <c r="J129" t="str">
+        <f t="shared" ref="J129" si="161">CONCATENATE(B129,B130,B131,B132,B133,B134,B135,B136)</f>
+        <v>10001001</v>
+      </c>
+      <c r="K129" t="str">
+        <f t="shared" ref="K129" si="162">CONCATENATE(C129,C130,C131,C132,C133,C134,C135,C136)</f>
+        <v>10001001</v>
+      </c>
+      <c r="L129" t="str">
+        <f t="shared" ref="L129" si="163">CONCATENATE(D129,D130,D131,D132,D133,D134,D135,D136)</f>
+        <v>10001001</v>
+      </c>
+      <c r="M129" t="str">
+        <f t="shared" ref="M129" si="164">CONCATENATE(E129,E130,E131,E132,E133,E134,E135,E136)</f>
+        <v>01111110</v>
+      </c>
+      <c r="N129" t="str">
+        <f t="shared" ref="N129" si="165">CONCATENATE(F129,F130,F131,F132,F133,F134,F135,F136)</f>
+        <v>00000000</v>
+      </c>
+      <c r="O129" t="str">
+        <f t="shared" ref="O129" si="166">CONCATENATE(G129,G130,G131,G132,G133,G134,G135,G136)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="130" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A130" s="23">
+        <v>1</v>
+      </c>
+      <c r="B130" s="3">
+        <v>0</v>
+      </c>
+      <c r="C130" s="3">
+        <v>0</v>
+      </c>
+      <c r="D130" s="3">
+        <v>0</v>
+      </c>
+      <c r="E130" s="24">
+        <v>1</v>
+      </c>
+      <c r="F130" s="3">
+        <v>0</v>
+      </c>
+      <c r="I130" s="13" t="str">
+        <f>CONCATENATE(A136,A135,A134,A133,A132,A131,A130,A129)</f>
+        <v>11111111</v>
+      </c>
+      <c r="J130" s="13" t="str">
+        <f t="shared" ref="J130" si="167">CONCATENATE(B136,B135,B134,B133,B132,B131,B130,B129)</f>
+        <v>10010001</v>
+      </c>
+      <c r="K130" s="13" t="str">
+        <f t="shared" ref="K130" si="168">CONCATENATE(C136,C135,C134,C133,C132,C131,C130,C129)</f>
+        <v>10010001</v>
+      </c>
+      <c r="L130" s="13" t="str">
+        <f t="shared" ref="L130" si="169">CONCATENATE(D136,D135,D134,D133,D132,D131,D130,D129)</f>
+        <v>10010001</v>
+      </c>
+      <c r="M130" s="13" t="str">
+        <f t="shared" ref="M130" si="170">CONCATENATE(E136,E135,E134,E133,E132,E131,E130,E129)</f>
+        <v>01111110</v>
+      </c>
+      <c r="N130" s="13" t="str">
+        <f t="shared" ref="N130" si="171">CONCATENATE(F136,F135,F134,F133,F132,F131,F130,F129)</f>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="131" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A131" s="23">
+        <v>1</v>
+      </c>
+      <c r="B131" s="3">
+        <v>0</v>
+      </c>
+      <c r="C131" s="3">
+        <v>0</v>
+      </c>
+      <c r="D131" s="3">
+        <v>0</v>
+      </c>
+      <c r="E131" s="23">
+        <v>1</v>
+      </c>
+      <c r="F131" s="3">
+        <v>0</v>
+      </c>
+      <c r="I131" s="5" t="str">
+        <f>MID(I129,1,8)</f>
+        <v>11111111</v>
+      </c>
+      <c r="J131" s="5" t="str">
+        <f t="shared" ref="J131:O131" si="172">MID(J129,1,8)</f>
+        <v>10001001</v>
+      </c>
+      <c r="K131" s="5" t="str">
+        <f t="shared" si="172"/>
+        <v>10001001</v>
+      </c>
+      <c r="L131" s="5" t="str">
+        <f t="shared" si="172"/>
+        <v>10001001</v>
+      </c>
+      <c r="M131" s="5" t="str">
+        <f t="shared" si="172"/>
+        <v>01111110</v>
+      </c>
+      <c r="N131" s="5" t="str">
+        <f t="shared" si="172"/>
+        <v>00000000</v>
+      </c>
+      <c r="O131" s="5" t="str">
+        <f t="shared" si="172"/>
+        <v/>
+      </c>
+    </row>
+    <row r="132" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A132" s="23">
+        <v>1</v>
+      </c>
+      <c r="B132" s="3">
+        <v>0</v>
+      </c>
+      <c r="C132" s="3">
+        <v>0</v>
+      </c>
+      <c r="D132" s="3">
+        <v>0</v>
+      </c>
+      <c r="E132" s="23">
+        <v>1</v>
+      </c>
+      <c r="F132" s="3">
+        <v>0</v>
+      </c>
+      <c r="I132" s="13" t="str">
+        <f>MID(I130,1,8)</f>
+        <v>11111111</v>
+      </c>
+      <c r="J132" s="13" t="str">
+        <f t="shared" ref="J132:N132" si="173">MID(J130,1,8)</f>
+        <v>10010001</v>
+      </c>
+      <c r="K132" s="13" t="str">
+        <f t="shared" si="173"/>
+        <v>10010001</v>
+      </c>
+      <c r="L132" s="13" t="str">
+        <f t="shared" si="173"/>
+        <v>10010001</v>
+      </c>
+      <c r="M132" s="13" t="str">
+        <f t="shared" si="173"/>
+        <v>01111110</v>
+      </c>
+      <c r="N132" s="13" t="str">
+        <f t="shared" si="173"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="133" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A133" s="23">
+        <v>1</v>
+      </c>
+      <c r="B133" s="23">
+        <v>1</v>
+      </c>
+      <c r="C133" s="23">
+        <v>1</v>
+      </c>
+      <c r="D133" s="23">
+        <v>1</v>
+      </c>
+      <c r="E133" s="23">
+        <v>1</v>
+      </c>
+      <c r="F133" s="3">
+        <v>0</v>
+      </c>
+      <c r="I133" s="6" t="str">
+        <f>BIN2HEX(I131,2)</f>
+        <v>FF</v>
+      </c>
+      <c r="J133" s="6" t="str">
+        <f t="shared" ref="J133:O133" si="174">BIN2HEX(J131,2)</f>
+        <v>89</v>
+      </c>
+      <c r="K133" s="6" t="str">
+        <f t="shared" si="174"/>
+        <v>89</v>
+      </c>
+      <c r="L133" s="6" t="str">
+        <f t="shared" si="174"/>
+        <v>89</v>
+      </c>
+      <c r="M133" s="6" t="str">
+        <f t="shared" si="174"/>
+        <v>7E</v>
+      </c>
+      <c r="N133" s="6" t="str">
+        <f t="shared" si="174"/>
+        <v>00</v>
+      </c>
+      <c r="O133" s="6" t="str">
+        <f t="shared" si="174"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="134" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A134" s="23">
+        <v>1</v>
+      </c>
+      <c r="B134" s="3">
+        <v>0</v>
+      </c>
+      <c r="C134" s="3">
+        <v>0</v>
+      </c>
+      <c r="D134" s="3">
+        <v>0</v>
+      </c>
+      <c r="E134" s="23">
+        <v>1</v>
+      </c>
+      <c r="F134" s="3">
+        <v>0</v>
+      </c>
+      <c r="I134" s="16" t="str">
+        <f t="shared" ref="I134:N134" si="175">BIN2HEX(I132,2)</f>
+        <v>FF</v>
+      </c>
+      <c r="J134" s="16" t="str">
+        <f t="shared" si="175"/>
+        <v>91</v>
+      </c>
+      <c r="K134" s="16" t="str">
+        <f t="shared" si="175"/>
+        <v>91</v>
+      </c>
+      <c r="L134" s="16" t="str">
+        <f t="shared" si="175"/>
+        <v>91</v>
+      </c>
+      <c r="M134" s="16" t="str">
+        <f t="shared" si="175"/>
+        <v>7E</v>
+      </c>
+      <c r="N134" s="16" t="str">
+        <f t="shared" si="175"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="135" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A135" s="23">
+        <v>1</v>
+      </c>
+      <c r="B135" s="3">
+        <v>0</v>
+      </c>
+      <c r="C135" s="3">
+        <v>0</v>
+      </c>
+      <c r="D135" s="3">
+        <v>0</v>
+      </c>
+      <c r="E135" s="23">
+        <v>1</v>
+      </c>
+      <c r="F135" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A136" s="23">
+        <v>1</v>
+      </c>
+      <c r="B136" s="23">
+        <v>1</v>
+      </c>
+      <c r="C136" s="23">
+        <v>1</v>
+      </c>
+      <c r="D136" s="23">
+        <v>1</v>
+      </c>
+      <c r="E136" s="3">
+        <v>0</v>
+      </c>
+      <c r="F136" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A137" s="3"/>
+      <c r="B137" s="3"/>
+      <c r="C137" s="3"/>
+      <c r="D137" s="3"/>
+      <c r="E137" s="3"/>
+      <c r="F137" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -3619,7 +5222,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="A9" sqref="A9:AN9"/>
     </sheetView>
   </sheetViews>
@@ -3739,48 +5342,48 @@
       <c r="AK8" s="10"/>
     </row>
     <row r="9" spans="1:40" ht="99" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="16"/>
-      <c r="S9" s="16"/>
-      <c r="T9" s="16"/>
-      <c r="U9" s="16"/>
-      <c r="V9" s="16"/>
-      <c r="W9" s="16"/>
-      <c r="X9" s="16"/>
-      <c r="Y9" s="16"/>
-      <c r="Z9" s="16"/>
-      <c r="AA9" s="16"/>
-      <c r="AB9" s="16"/>
-      <c r="AC9" s="16"/>
-      <c r="AD9" s="16"/>
-      <c r="AE9" s="16"/>
-      <c r="AF9" s="16"/>
-      <c r="AG9" s="16"/>
-      <c r="AH9" s="16"/>
-      <c r="AI9" s="16"/>
-      <c r="AJ9" s="16"/>
-      <c r="AK9" s="16"/>
-      <c r="AL9" s="16"/>
-      <c r="AM9" s="16"/>
-      <c r="AN9" s="16"/>
+      <c r="A9" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="22"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="22"/>
+      <c r="U9" s="22"/>
+      <c r="V9" s="22"/>
+      <c r="W9" s="22"/>
+      <c r="X9" s="22"/>
+      <c r="Y9" s="22"/>
+      <c r="Z9" s="22"/>
+      <c r="AA9" s="22"/>
+      <c r="AB9" s="22"/>
+      <c r="AC9" s="22"/>
+      <c r="AD9" s="22"/>
+      <c r="AE9" s="22"/>
+      <c r="AF9" s="22"/>
+      <c r="AG9" s="22"/>
+      <c r="AH9" s="22"/>
+      <c r="AI9" s="22"/>
+      <c r="AJ9" s="22"/>
+      <c r="AK9" s="22"/>
+      <c r="AL9" s="22"/>
+      <c r="AM9" s="22"/>
+      <c r="AN9" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>